<commit_message>
fixed bad character spreadsheet formatting
</commit_message>
<xml_diff>
--- a/Book-List-Final-NONA.xlsx
+++ b/Book-List-Final-NONA.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="999">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="1000">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -823,7 +823,7 @@
     <t xml:space="preserve">NH/H/H/H/H/NH/NH/H</t>
   </si>
   <si>
-    <t xml:space="preserve">spider;tiny black creature/Hank Chief; pirate chief/Ben Buckle/Percy Patch/Peg Polkadot/mouse;furry creature/rabbit;creature with long ears,pirates</t>
+    <t xml:space="preserve">spider;tiny black creature/Hank Chief; pirate chief/Ben Buckle/Percy Patch/Peg Polkadot/mouse;furry creature/rabbit;creature with long ears/pirates</t>
   </si>
   <si>
     <t xml:space="preserve">Tabby McTat</t>
@@ -928,7 +928,7 @@
     <t xml:space="preserve">H/H/NH/NH/H/NH/NH/NH/NH/NH/H/H/H/H/H/H/NH/H/H/NH/H/H/H/H/H/H</t>
   </si>
   <si>
-    <t xml:space="preserve">pirate chief;chief/Goldilocks/bears/baby bear/Sir Percy Pilkington/dragon/Rowena Reddalot/birds;each bird/owl/rook/girl/green men/mother;mum/spaceman/thief/king/sheep/Lady Mary/Lady/daughter;her daughter Featherington/Crocodile/Queen/Bunn Twins/Blacksmith/cakemakers/ghost</t>
+    <t xml:space="preserve">pirate chief;chief/Goldilocks/bears/baby bear/Sir Percy Pilkington/dragon/Rowena Reddalot/birds;each bird/owl/rook/girl/green men/mother;mum/spaceman/thief/king/sheep/Lady Mary/Lady Featherington/Crocodile/Queen/Bunn Twins/Blacksmith/cakemakers/ghost/daughter;her daughter</t>
   </si>
   <si>
     <t xml:space="preserve">Potentially odd for language analysis at sentence level as lots of run on sentences. Ghost here marked as human, as is santa.</t>
@@ -1003,7 +1003,7 @@
     <t xml:space="preserve">Sid</t>
   </si>
   <si>
-    <t xml:space="preserve">F/M/M/F/M/F/NGS/NGS </t>
+    <t xml:space="preserve">F/M/M/F/M/F/NGS</t>
   </si>
   <si>
     <t xml:space="preserve">Madame Murple/Pete/Little Billy/Grandma/firefighter/ladies/the crowd;the street</t>
@@ -2129,6 +2129,9 @@
   </si>
   <si>
     <t xml:space="preserve">NH/NH/NH/NH/NH/NH/NH/NH/NH/NH/NH/NH/NH/NH/NH/NH/NH/H/H/H/NH/NH/NH/H/H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dogs/bears/monkeys/mice/whales/rabbits/camels/kangeroos/elephants/peacocks/skunks/squid/rhinos/tortoises/pigs/pythons/clowns/princess/snowman/pirates/trolls/bats/martians/babies/The judge;judge</t>
   </si>
   <si>
     <t xml:space="preserve">Bottoms Up!</t>
@@ -3026,7 +3029,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -3055,6 +3058,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -3126,7 +3135,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3155,7 +3164,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3163,7 +3176,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3246,8 +3259,8 @@
   </sheetPr>
   <dimension ref="A1:Q207"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M178" colorId="64" zoomScale="274" zoomScaleNormal="274" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="O185" activeCellId="0" sqref="O185"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M53" colorId="64" zoomScale="274" zoomScaleNormal="274" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M59" activeCellId="0" sqref="M59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10098,8 +10111,8 @@
       <c r="N138" s="2" t="s">
         <v>702</v>
       </c>
-      <c r="O138" s="2" t="s">
-        <v>555</v>
+      <c r="O138" s="7" t="s">
+        <v>703</v>
       </c>
       <c r="P138" s="2"/>
       <c r="Q138" s="2" t="n">
@@ -10111,7 +10124,7 @@
         <v>138</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>703</v>
+        <v>704</v>
       </c>
       <c r="C139" s="2" t="s">
         <v>700</v>
@@ -10144,13 +10157,13 @@
         <v>41</v>
       </c>
       <c r="M139" s="2" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="N139" s="2" t="s">
         <v>32</v>
       </c>
       <c r="O139" s="2" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="P139" s="2"/>
       <c r="Q139" s="2" t="n">
@@ -10162,10 +10175,10 @@
         <v>139</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>258</v>
@@ -10192,19 +10205,19 @@
         <v>32</v>
       </c>
       <c r="L140" s="2" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="M140" s="2" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="N140" s="2" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="O140" s="2" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="P140" s="2" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="Q140" s="2" t="n">
         <v>2013</v>
@@ -10215,10 +10228,10 @@
         <v>140</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>28</v>
@@ -10241,19 +10254,19 @@
         <v>32</v>
       </c>
       <c r="L141" s="2" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="M141" s="2" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="N141" s="2" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="O141" s="2" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="P141" s="2" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="Q141" s="2" t="n">
         <v>2018</v>
@@ -10264,10 +10277,10 @@
         <v>141</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>19</v>
@@ -10290,19 +10303,19 @@
         <v>32</v>
       </c>
       <c r="L142" s="2" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="M142" s="2" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="N142" s="2" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="O142" s="2" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="P142" s="2" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="Q142" s="2" t="n">
         <v>2014</v>
@@ -10313,10 +10326,10 @@
         <v>142</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>28</v>
@@ -10339,16 +10352,16 @@
         <v>26</v>
       </c>
       <c r="L143" s="2" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="M143" s="2" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="N143" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O143" s="2" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="P143" s="2"/>
       <c r="Q143" s="2" t="n">
@@ -10360,10 +10373,10 @@
         <v>143</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>28</v>
@@ -10390,7 +10403,7 @@
         <v>26</v>
       </c>
       <c r="L144" s="2" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="M144" s="2" t="s">
         <v>40</v>
@@ -10399,7 +10412,7 @@
         <v>26</v>
       </c>
       <c r="O144" s="2" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="P144" s="2"/>
       <c r="Q144" s="2" t="n">
@@ -10411,10 +10424,10 @@
         <v>144</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>258</v>
@@ -10441,16 +10454,16 @@
         <v>32</v>
       </c>
       <c r="L145" s="2" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="M145" s="2" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="N145" s="2" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="O145" s="2" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="P145" s="2"/>
       <c r="Q145" s="2" t="n">
@@ -10462,7 +10475,7 @@
         <v>145</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="C146" s="2" t="s">
         <v>700</v>
@@ -10491,13 +10504,13 @@
       <c r="K146" s="2"/>
       <c r="L146" s="2"/>
       <c r="M146" s="2" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="N146" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O146" s="2" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="P146" s="2"/>
       <c r="Q146" s="2" t="n">
@@ -10509,10 +10522,10 @@
         <v>146</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>258</v>
@@ -10538,13 +10551,13 @@
         <v>111</v>
       </c>
       <c r="M147" s="2" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="N147" s="2" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="O147" s="2" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="P147" s="2"/>
       <c r="Q147" s="2" t="n">
@@ -10556,10 +10569,10 @@
         <v>147</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>28</v>
@@ -10582,7 +10595,7 @@
         <v>26</v>
       </c>
       <c r="L148" s="2" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="M148" s="2" t="s">
         <v>206</v>
@@ -10591,7 +10604,7 @@
         <v>383</v>
       </c>
       <c r="O148" s="2" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="P148" s="2"/>
       <c r="Q148" s="2" t="n">
@@ -10603,10 +10616,10 @@
         <v>148</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>206</v>
@@ -10629,7 +10642,7 @@
         <v>32</v>
       </c>
       <c r="L149" s="2" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="M149" s="2" t="s">
         <v>258</v>
@@ -10638,10 +10651,10 @@
         <v>435</v>
       </c>
       <c r="O149" s="2" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="P149" s="2" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="Q149" s="2" t="n">
         <v>2020</v>
@@ -10652,10 +10665,10 @@
         <v>149</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>28</v>
@@ -10678,16 +10691,16 @@
         <v>32</v>
       </c>
       <c r="L150" s="2" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="M150" s="2" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="N150" s="2" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="O150" s="2" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="P150" s="2"/>
       <c r="Q150" s="2" t="n">
@@ -10699,10 +10712,10 @@
         <v>150</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>19</v>
@@ -10736,7 +10749,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>246</v>
@@ -10762,19 +10775,19 @@
         <v>369</v>
       </c>
       <c r="L152" s="2" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="M152" s="2" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="N152" s="2" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="O152" s="2" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="P152" s="2" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="Q152" s="2" t="n">
         <v>2018</v>
@@ -10785,7 +10798,7 @@
         <v>152</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="C153" s="2" t="s">
         <v>246</v>
@@ -10811,19 +10824,19 @@
         <v>32</v>
       </c>
       <c r="L153" s="2" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="M153" s="2" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="N153" s="2" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="O153" s="2" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="P153" s="2" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="Q153" s="2" t="n">
         <v>2010</v>
@@ -10834,7 +10847,7 @@
         <v>153</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="C154" s="2" t="s">
         <v>246</v>
@@ -10860,16 +10873,16 @@
         <v>45</v>
       </c>
       <c r="L154" s="2" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="M154" s="2" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="N154" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O154" s="4" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="P154" s="2"/>
       <c r="Q154" s="2" t="n">
@@ -10881,7 +10894,7 @@
         <v>154</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="C155" s="2" t="s">
         <v>246</v>
@@ -10907,16 +10920,16 @@
         <v>26</v>
       </c>
       <c r="L155" s="2" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="M155" s="2" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="N155" s="2" t="s">
         <v>130</v>
       </c>
       <c r="O155" s="2" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="P155" s="2"/>
       <c r="Q155" s="2" t="n">
@@ -10928,7 +10941,7 @@
         <v>155</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="C156" s="2" t="s">
         <v>246</v>
@@ -10954,16 +10967,16 @@
         <v>26</v>
       </c>
       <c r="L156" s="2" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="M156" s="2" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="N156" s="2" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="O156" s="2" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="P156" s="2"/>
       <c r="Q156" s="2" t="n">
@@ -10975,7 +10988,7 @@
         <v>156</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="C157" s="2" t="s">
         <v>246</v>
@@ -11001,16 +11014,16 @@
         <v>26</v>
       </c>
       <c r="L157" s="2" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="M157" s="2" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="N157" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O157" s="4" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="P157" s="2"/>
       <c r="Q157" s="2" t="n">
@@ -11022,7 +11035,7 @@
         <v>157</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="C158" s="2" t="s">
         <v>246</v>
@@ -11048,16 +11061,16 @@
         <v>26</v>
       </c>
       <c r="L158" s="2" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="M158" s="2" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="N158" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O158" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="P158" s="2"/>
       <c r="Q158" s="2" t="n">
@@ -11069,7 +11082,7 @@
         <v>158</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="C159" s="2" t="s">
         <v>246</v>
@@ -11095,16 +11108,16 @@
         <v>26</v>
       </c>
       <c r="L159" s="2" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="M159" s="2" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="N159" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O159" s="2" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="P159" s="2"/>
       <c r="Q159" s="2" t="n">
@@ -11116,7 +11129,7 @@
         <v>159</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>246</v>
@@ -11147,7 +11160,7 @@
         <v>26</v>
       </c>
       <c r="O160" s="2" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="P160" s="2"/>
       <c r="Q160" s="2" t="n">
@@ -11159,7 +11172,7 @@
         <v>160</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="C161" s="2" t="s">
         <v>246</v>
@@ -11185,16 +11198,16 @@
         <v>32</v>
       </c>
       <c r="L161" s="2" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="M161" s="2" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="N161" s="2" t="s">
         <v>32</v>
       </c>
       <c r="O161" s="2" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="P161" s="2"/>
       <c r="Q161" s="2" t="n">
@@ -11206,7 +11219,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="C162" s="2" t="s">
         <v>246</v>
@@ -11232,7 +11245,7 @@
         <v>45</v>
       </c>
       <c r="L162" s="2" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="M162" s="2" t="s">
         <v>154</v>
@@ -11241,7 +11254,7 @@
         <v>399</v>
       </c>
       <c r="O162" s="2" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="P162" s="2"/>
       <c r="Q162" s="2" t="n">
@@ -11253,7 +11266,7 @@
         <v>162</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="C163" s="2" t="s">
         <v>246</v>
@@ -11279,16 +11292,16 @@
         <v>26</v>
       </c>
       <c r="L163" s="2" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="M163" s="2" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="N163" s="2" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="O163" s="2" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="P163" s="2"/>
       <c r="Q163" s="2" t="n">
@@ -11300,7 +11313,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="C164" s="2" t="s">
         <v>246</v>
@@ -11326,19 +11339,19 @@
         <v>26</v>
       </c>
       <c r="L164" s="2" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="M164" s="2" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="N164" s="2" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="O164" s="2" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="P164" s="2" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="Q164" s="2" t="n">
         <v>2010</v>
@@ -11349,7 +11362,7 @@
         <v>164</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="C165" s="2" t="s">
         <v>246</v>
@@ -11375,16 +11388,16 @@
         <v>45</v>
       </c>
       <c r="L165" s="2" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="M165" s="2" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="N165" s="2" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="O165" s="2" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="P165" s="2"/>
       <c r="Q165" s="2" t="n">
@@ -11396,7 +11409,7 @@
         <v>165</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>246</v>
@@ -11422,16 +11435,16 @@
         <v>32</v>
       </c>
       <c r="L166" s="2" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="M166" s="2" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="N166" s="2" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="O166" s="2" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="P166" s="2"/>
       <c r="Q166" s="2" t="n">
@@ -11443,7 +11456,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="C167" s="2" t="s">
         <v>246</v>
@@ -11469,19 +11482,19 @@
         <v>32</v>
       </c>
       <c r="L167" s="2" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="M167" s="2" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="N167" s="2" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="O167" s="2" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="P167" s="2" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="Q167" s="2" t="n">
         <v>2012</v>
@@ -11521,13 +11534,13 @@
         <v>388</v>
       </c>
       <c r="M168" s="2" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="N168" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O168" s="2" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="P168" s="2"/>
       <c r="Q168" s="2" t="n">
@@ -11539,7 +11552,7 @@
         <v>168</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>387</v>
@@ -11565,19 +11578,19 @@
         <v>45</v>
       </c>
       <c r="L169" s="2" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="M169" s="2" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="N169" s="2" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="O169" s="2" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="P169" s="2" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="Q169" s="2" t="n">
         <v>2016</v>
@@ -11588,10 +11601,10 @@
         <v>169</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>28</v>
@@ -11614,19 +11627,19 @@
         <v>45</v>
       </c>
       <c r="L170" s="2" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="M170" s="2" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="N170" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O170" s="2" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="P170" s="2" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="Q170" s="2" t="n">
         <v>2013</v>
@@ -11637,10 +11650,10 @@
         <v>170</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>28</v>
@@ -11663,16 +11676,16 @@
         <v>45</v>
       </c>
       <c r="L171" s="2" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="M171" s="2" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="N171" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O171" s="2" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="P171" s="2"/>
       <c r="Q171" s="2" t="n">
@@ -11684,10 +11697,10 @@
         <v>171</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>28</v>
@@ -11719,7 +11732,7 @@
         <v>26</v>
       </c>
       <c r="O172" s="2" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="P172" s="2"/>
       <c r="Q172" s="2" t="n">
@@ -11731,10 +11744,10 @@
         <v>172</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>28</v>
@@ -11757,7 +11770,7 @@
         <v>45</v>
       </c>
       <c r="L173" s="2" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="M173" s="2" t="s">
         <v>58</v>
@@ -11766,7 +11779,7 @@
         <v>26</v>
       </c>
       <c r="O173" s="2" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="P173" s="2"/>
       <c r="Q173" s="2" t="n">
@@ -11778,10 +11791,10 @@
         <v>173</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>28</v>
@@ -11804,7 +11817,7 @@
         <v>45</v>
       </c>
       <c r="L174" s="2" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="M174" s="2" t="s">
         <v>73</v>
@@ -11813,7 +11826,7 @@
         <v>45</v>
       </c>
       <c r="O174" s="2" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="P174" s="2"/>
       <c r="Q174" s="2" t="n">
@@ -11825,7 +11838,7 @@
         <v>174</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="C175" s="2" t="s">
         <v>387</v>
@@ -11851,16 +11864,16 @@
         <v>26</v>
       </c>
       <c r="L175" s="2" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="M175" s="2" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="N175" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O175" s="2" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="P175" s="2"/>
       <c r="Q175" s="2" t="n">
@@ -11872,10 +11885,10 @@
         <v>175</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>28</v>
@@ -11898,16 +11911,16 @@
         <v>45</v>
       </c>
       <c r="L176" s="2" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="M176" s="2" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="N176" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O176" s="2" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="P176" s="2"/>
       <c r="Q176" s="2" t="n">
@@ -11919,10 +11932,10 @@
         <v>176</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>28</v>
@@ -11944,16 +11957,16 @@
       <c r="K177" s="2"/>
       <c r="L177" s="2"/>
       <c r="M177" s="2" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="N177" s="2" t="s">
         <v>32</v>
       </c>
       <c r="O177" s="2" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="P177" s="2" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="Q177" s="2" t="n">
         <v>2019</v>
@@ -11964,10 +11977,10 @@
         <v>177</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>28</v>
@@ -11990,16 +12003,16 @@
         <v>32</v>
       </c>
       <c r="L178" s="2" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="M178" s="2" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="N178" s="2" t="s">
         <v>32</v>
       </c>
       <c r="O178" s="2" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="P178" s="2"/>
       <c r="Q178" s="2" t="n">
@@ -12011,10 +12024,10 @@
         <v>178</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>28</v>
@@ -12037,16 +12050,16 @@
         <v>32</v>
       </c>
       <c r="L179" s="2" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="M179" s="2" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="N179" s="2" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="O179" s="2" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="P179" s="2"/>
       <c r="Q179" s="2" t="n">
@@ -12058,10 +12071,10 @@
         <v>179</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>28</v>
@@ -12084,19 +12097,19 @@
         <v>32</v>
       </c>
       <c r="L180" s="2" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="M180" s="2" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="N180" s="2" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="O180" s="2" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="P180" s="2" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="Q180" s="2" t="n">
         <v>2019</v>
@@ -12107,10 +12120,10 @@
         <v>180</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>28</v>
@@ -12137,16 +12150,16 @@
         <v>45</v>
       </c>
       <c r="L181" s="2" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="M181" s="2" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="N181" s="2" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="O181" s="2" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="P181" s="2"/>
       <c r="Q181" s="2" t="n">
@@ -12158,10 +12171,10 @@
         <v>181</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="D182" s="2" t="s">
         <v>258</v>
@@ -12188,19 +12201,19 @@
         <v>26</v>
       </c>
       <c r="L182" s="2" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="M182" s="2" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="N182" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O182" s="2" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="P182" s="2" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="Q182" s="2" t="n">
         <v>2014</v>
@@ -12211,17 +12224,17 @@
         <v>182</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="D183" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E183" s="2"/>
       <c r="F183" s="2" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="G183" s="2" t="n">
         <v>6</v>
@@ -12239,16 +12252,16 @@
         <v>45</v>
       </c>
       <c r="L183" s="2" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="M183" s="2" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="N183" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O183" s="2" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="P183" s="2"/>
       <c r="Q183" s="2" t="n">
@@ -12260,10 +12273,10 @@
         <v>183</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>19</v>
@@ -12286,16 +12299,16 @@
         <v>32</v>
       </c>
       <c r="L184" s="2" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="M184" s="2" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="N184" s="2" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="O184" s="2" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="P184" s="2"/>
       <c r="Q184" s="2" t="n">
@@ -12307,10 +12320,10 @@
         <v>184</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="D185" s="1" t="s">
         <v>28</v>
@@ -12334,10 +12347,10 @@
         <v>185</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="D186" s="2" t="s">
         <v>19</v>
@@ -12364,19 +12377,19 @@
         <v>369</v>
       </c>
       <c r="L186" s="2" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="M186" s="2" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="N186" s="2" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="O186" s="2" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="P186" s="2" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="Q186" s="2" t="n">
         <v>2020</v>
@@ -12387,10 +12400,10 @@
         <v>186</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="D187" s="2" t="s">
         <v>28</v>
@@ -12417,16 +12430,16 @@
         <v>26</v>
       </c>
       <c r="L187" s="2" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="M187" s="2" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="N187" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O187" s="2" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="P187" s="2"/>
       <c r="Q187" s="2" t="n">
@@ -12438,10 +12451,10 @@
         <v>187</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="D188" s="2" t="s">
         <v>258</v>
@@ -12471,13 +12484,13 @@
         <v>352</v>
       </c>
       <c r="M188" s="2" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="N188" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O188" s="2" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="P188" s="2"/>
       <c r="Q188" s="2" t="n">
@@ -12489,10 +12502,10 @@
         <v>188</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="D189" s="2" t="s">
         <v>258</v>
@@ -12519,16 +12532,16 @@
         <v>26</v>
       </c>
       <c r="L189" s="2" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="M189" s="2" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="N189" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O189" s="2" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="P189" s="2"/>
       <c r="Q189" s="2" t="n">
@@ -12540,10 +12553,10 @@
         <v>189</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="D190" s="2" t="s">
         <v>28</v>
@@ -12566,16 +12579,16 @@
         <v>32</v>
       </c>
       <c r="L190" s="2" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="M190" s="2" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="N190" s="2" t="s">
         <v>261</v>
       </c>
       <c r="O190" s="2" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="P190" s="2"/>
       <c r="Q190" s="2" t="n">
@@ -12587,10 +12600,10 @@
         <v>190</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>258</v>
@@ -12617,19 +12630,19 @@
         <v>26</v>
       </c>
       <c r="L191" s="2" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="M191" s="2" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="N191" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O191" s="2" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="P191" s="2" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="Q191" s="2" t="n">
         <v>2016</v>
@@ -12640,10 +12653,10 @@
         <v>191</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>19</v>
@@ -12666,16 +12679,16 @@
         <v>361</v>
       </c>
       <c r="L192" s="2" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="M192" s="2" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="N192" s="2" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="O192" s="2" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="P192" s="2"/>
       <c r="Q192" s="2" t="n">
@@ -12687,17 +12700,17 @@
         <v>192</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="D193" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E193" s="2"/>
       <c r="F193" s="2" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="G193" s="2" t="n">
         <v>8</v>
@@ -12715,19 +12728,19 @@
         <v>45</v>
       </c>
       <c r="L193" s="2" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="M193" s="2" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="N193" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O193" s="2" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="P193" s="2" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="Q193" s="2" t="n">
         <v>2012</v>
@@ -12738,10 +12751,10 @@
         <v>193</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>258</v>
@@ -12768,16 +12781,16 @@
         <v>26</v>
       </c>
       <c r="L194" s="2" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="M194" s="2" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="N194" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O194" s="2" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="P194" s="2"/>
       <c r="Q194" s="2" t="n">
@@ -12789,10 +12802,10 @@
         <v>194</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>258</v>
@@ -12819,16 +12832,16 @@
         <v>26</v>
       </c>
       <c r="L195" s="2" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="M195" s="2" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="N195" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O195" s="2" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="P195" s="2"/>
       <c r="Q195" s="2" t="n">
@@ -12840,10 +12853,10 @@
         <v>195</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>19</v>
@@ -12870,16 +12883,16 @@
         <v>45</v>
       </c>
       <c r="L196" s="2" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="M196" s="2" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="N196" s="2" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="O196" s="2" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="P196" s="2"/>
       <c r="Q196" s="2" t="n">
@@ -12891,10 +12904,10 @@
         <v>196</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="D197" s="2" t="s">
         <v>19</v>
@@ -12921,16 +12934,16 @@
         <v>45</v>
       </c>
       <c r="L197" s="2" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="M197" s="2" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="N197" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O197" s="2" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="P197" s="2"/>
       <c r="Q197" s="2" t="n">
@@ -12942,10 +12955,10 @@
         <v>197</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="D198" s="2" t="s">
         <v>28</v>
@@ -12972,16 +12985,16 @@
         <v>32</v>
       </c>
       <c r="L198" s="2" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="M198" s="2" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="N198" s="2" t="s">
         <v>565</v>
       </c>
       <c r="O198" s="2" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="P198" s="2"/>
       <c r="Q198" s="2" t="n">
@@ -12993,10 +13006,10 @@
         <v>198</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="D199" s="2" t="s">
         <v>78</v>
@@ -13023,16 +13036,16 @@
         <v>45</v>
       </c>
       <c r="L199" s="2" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="M199" s="2" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="N199" s="2" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="O199" s="2" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="P199" s="2"/>
       <c r="Q199" s="2" t="n">
@@ -13044,10 +13057,10 @@
         <v>199</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="D200" s="2" t="s">
         <v>19</v>
@@ -13074,16 +13087,16 @@
         <v>361</v>
       </c>
       <c r="L200" s="2" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="M200" s="2" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="N200" s="2" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="O200" s="2" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="P200" s="2"/>
       <c r="Q200" s="2" t="n">
@@ -13095,10 +13108,10 @@
         <v>200</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="D201" s="2" t="s">
         <v>19</v>
@@ -13121,16 +13134,16 @@
         <v>32</v>
       </c>
       <c r="L201" s="2" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="M201" s="2" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="N201" s="2" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="O201" s="2" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="P201" s="2"/>
       <c r="Q201" s="2" t="n">
@@ -13142,10 +13155,10 @@
         <v>201</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="D202" s="2" t="s">
         <v>19</v>
@@ -13162,13 +13175,13 @@
         <v>24</v>
       </c>
       <c r="J202" s="2" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="K202" s="2" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="L202" s="2" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="M202" s="2" t="s">
         <v>19</v>
@@ -13177,7 +13190,7 @@
         <v>26</v>
       </c>
       <c r="O202" s="2" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="P202" s="2"/>
       <c r="Q202" s="2" t="n">
@@ -13185,24 +13198,24 @@
       </c>
     </row>
     <row r="203" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C203" s="7"/>
-      <c r="D203" s="7"/>
+      <c r="C203" s="8"/>
+      <c r="D203" s="8"/>
     </row>
     <row r="204" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C204" s="8"/>
-      <c r="D204" s="8"/>
+      <c r="C204" s="9"/>
+      <c r="D204" s="9"/>
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C206" s="9" t="s">
-        <v>997</v>
-      </c>
-      <c r="D206" s="9"/>
+      <c r="C206" s="10" t="s">
+        <v>998</v>
+      </c>
+      <c r="D206" s="10"/>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C207" s="9" t="s">
-        <v>998</v>
-      </c>
-      <c r="D207" s="9"/>
+      <c r="C207" s="10" t="s">
+        <v>999</v>
+      </c>
+      <c r="D207" s="10"/>
       <c r="E207" s="0" t="n">
         <f aca="false">SUM(E2:E203)</f>
         <v>334.19</v>

</xml_diff>

<commit_message>
fixed gender typos in spreadsheet
</commit_message>
<xml_diff>
--- a/Book-List-Final-NONA.xlsx
+++ b/Book-List-Final-NONA.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="1000">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2135" uniqueCount="1001">
   <si>
     <t xml:space="preserve">Number</t>
   </si>
@@ -520,10 +520,10 @@
     <t xml:space="preserve">Elmer and the Lost Teddy</t>
   </si>
   <si>
-    <t xml:space="preserve">M/F/M/NGS/NGS/NGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Baby Elephant/Baby Elephant's mother/Wilbur/Lion/Tiger/Teddy</t>
+    <t xml:space="preserve">M/F/M/NGS/NGS/NGS/NGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Baby Elephant/Baby Elephant's mother/Wilbur/Lion/Tiger/Teddy/All the young ones</t>
   </si>
   <si>
     <t xml:space="preserve">Elmer and the Wind</t>
@@ -532,7 +532,7 @@
     <t xml:space="preserve">M/NGS/NGS/NGS/NGS</t>
   </si>
   <si>
-    <t xml:space="preserve">Wilbur/bird;birds/elephants;elephant/lion/animals;other animals</t>
+    <t xml:space="preserve">Wilbur/bird;birds/elephants;elephant/lion/animals;the other animals</t>
   </si>
   <si>
     <t xml:space="preserve">I have conflated the single and plural versions of bird and elephant, as there is no distinction made between them in the text in terms of character, if that makes sense. It's a grey area, I can refine this and justify it.</t>
@@ -1021,192 +1021,195 @@
     <t xml:space="preserve">cavemen</t>
   </si>
   <si>
-    <t xml:space="preserve">M/M/NGS/NGS/NGS/M</t>
+    <t xml:space="preserve">M/M/NGS/NGS/NGS/M/M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H/NH/NH/NH/NH/NH/H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mankind/Tyrannosaurus rex;T-Rex/Triceratops/Styracosaurus/Stegosaurus/Diplodocus/man</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kipper's Toybox</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mick Inkpen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kipper</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M/M/NGS/M/NGS/NGS/NGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Owl/Sock Thing/Rabbit/Mr Snake/Slipper/Hippopotamus/mice;their babies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Captain Duck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Duck</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M/M/NGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Goat/Frog/Sheep</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You Choose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nick Sharratt and Pippa Goodheart</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is second person address. There are lots of clearly gendered pictures, including two recurring characters who are shown speaking with speech bubbles. I haven't included the dialogue from those bubbles here, as they are part of the picture and we're not assuming gender based on image alone for this project. The characters are unnamed. Could be an interesting source for a study on pictures at a later date.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We're Going On A Lion Hunt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">David Axtell</t>
+  </si>
+  <si>
+    <t xml:space="preserve">we; we're</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Pirates Next Door</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jonny Duddle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matilda; Tilda</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M/M/F/M/F/F/F/F/M/F/F/M/F/F/M/F/F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pirate boy; Jim Lad/Grandpa/Mum/Dad/teacher/Mrs Bumble/Mrs Pinky/Miss Divine/Mr Shaw/Miss Yates/Miss Yates/Postman/Mrs Snucks/Mrs Plumb/Mr Brown/Mrs Bevan/Nugget</t>
+  </si>
+  <si>
+    <t xml:space="preserve">There are two lots of Mum and Dad here. For ease of analysis I have conflated them into one gender token per word. This is not common - I think the only book in this collection in which that issue has come up.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Jolly Postman or Other People's Letters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Allan Ahlberg and Janet Ahlberg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Postman</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M/F/M/F/F/M/F/M/M/F/F/M/M/F/F/F/F/M/F/F/M/M/NGS/M/M/NGS/F/NGS/M/NGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NH/NH/NH/H/H/H/H/H/H/H/NH/H/H/H/H/H/H/H/H/H/NH/H/NH/H/NH/H/H/H/H/H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr Bear/Mrs Bear/Baby Bear;bear/Goldilocks/Mummy/Daddy/Witch/little boy/Giant Bigg/Mum/hen/bloke/Jack/Cinderella/Stepmother/stepsisters/fairy godmother/prince/grandma;lady/Miss Riding Hood/Mr Wolf/Woodcutter/King's horses/King's men/pigs/H Meeny/Mrs Banting;Mrs Bunting/Baby/baker's man/Miss Riding-Hood's Solicitors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Another stories in stories one. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dogger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shirley Hughes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H/NH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dave/Dogger</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F/M/F/M/F/M/F/F</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H/H/H/H/H/NH/H/H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bella/Joe/Mum/Dad/Barbara/Teddy Bear;Teddy/lady/Little girl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Might be counter stereotypical..? Dave really loves his toy, and his sister sort of saves the day...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How to Catch a Star</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oliver Jeffers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seagull </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good example of how normal everyday actions are storyworthy when a boy does them.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lost and Found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">boy/penguin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NGS/NGS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NH/NH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">birds/whales and dolphins</t>
+  </si>
+  <si>
+    <t xml:space="preserve">An odd little book, a story/colouring book with various promtps about what to draw.  Enough of a storybook to make our list I think. It is direct address but story follows 'boy and penguin' so have lableed those as protagonnists.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supertato Veggies Assemble</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sue Hendra and Paul Linnet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supertato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M/NGS/NGS/NGS/NGS/NGS/NGS/NGS/NGS/NGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Evil Pea/Pepper/Pear/Melon/Carrot/Lolly;the other/Cucumber/Broccoli/Tomato/Aubergine</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The Lighthouse Keeper's Lunch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ronda and David Armitage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr. Grinling; Mr Grinling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F/M/M/M/M/M</t>
   </si>
   <si>
     <t xml:space="preserve">H/NH/NH/NH/NH/NH</t>
   </si>
   <si>
-    <t xml:space="preserve">mankind/Tyrannosaurus rex;T-Rex/Triceratops/Styracosaurus/Stegosaurus/Diplodocus  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kipper's Toybox</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mick Inkpen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M  </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Kipper</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M/M/NGS/M/NGS/NGS/NGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Owl/Sock Thing/Rabbit/Mr Snake/Slipper/Hippopotamus/mice;their babies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Captain Duck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Duck</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M/M/NGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Goat/Frog/Sheep</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You Choose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nick Sharratt and Pippa Goodheart</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This is second person address. There are lots of clearly gendered pictures, including two recurring characters who are shown speaking with speech bubbles. I haven't included the dialogue from those bubbles here, as they are part of the picture and we're not assuming gender based on image alone for this project. The characters are unnamed. Could be an interesting source for a study on pictures at a later date.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We're Going On A Lion Hunt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">David Axtell</t>
-  </si>
-  <si>
-    <t xml:space="preserve">we; we're</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lion</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Pirates Next Door</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Jonny Duddle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Matilda; Tilda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M/M/F/M/F/F/F/F/M/F/F/M/F/F/M/F/F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pirate boy; Jim Lad/Grandpa/Mum/Dad/teacher/Mrs Bumble/Mrs Pinky/Miss Divine/Mr Shaw/Miss Yates/Miss Yates/Postman/Mrs Snucks/Mrs Plumb/Mr Brown/Mrs Bevan/Nugget</t>
-  </si>
-  <si>
-    <t xml:space="preserve">There are two lots of Mum and Dad here. For ease of analysis I have conflated them into one gender token per word. This is not common - I think the only book in this collection in which that issue has come up.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Jolly Postman or Other People's Letters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Allan Ahlberg and Janet Ahlberg</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Postman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M/F/M/F/F/M/F/M/M/F/F/M/M/F/F/F/F/M/F/F/M/M/NGS/M/M/NGS/F/NGS/M/NGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NH/NH/NH/H/H/H/H/H/H/H/NH/H/H/H/H/H/H/H/H/H/NH/H/NH/H/NH/H/H/H/H/H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mr Bear/Mrs Bear/Baby Bear;bear/Goldilocks/Mummy/Daddy/Witch/little boy/Giant Bigg/Mum/hen/bloke/Jack/Cinderella/Stepmother/stepsisters/fairy godmother/prince/grandma;lady/Miss Riding Hood/Mr Wolf/Woodcutter/King's horses/King's men/pigs/H Meeny/Mrs Banting;Mrs Bunting/Baby/baker's man/Miss Riding-Hood's Solicitors</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Another stories in stories one. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dogger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shirley Hughes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H/NH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dave/Dogger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F/M/F/M/F/M/F/F</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H/H/H/H/H/NH/H/H</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bella/Joe/Mum/Dad/Barbara/Teddy Bear;Teddy/lady/Little girl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Might be counter stereotypical..? Dave really loves his toy, and his sister sort of saves the day...</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How to Catch a Star</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oliver Jeffers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Seagull </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Good example of how normal everyday actions are storyworthy when a boy does them.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lost and Found</t>
-  </si>
-  <si>
-    <t xml:space="preserve">boy/penguin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NGS/NGS </t>
-  </si>
-  <si>
-    <t xml:space="preserve">NH/NH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">birds/whales and dolphins</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An odd little book, a story/colouring book with various promtps about what to draw.  Enough of a storybook to make our list I think. It is direct address but story follows 'boy and penguin' so have lableed those as protagonnists.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supertato Veggies Assemble</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sue Hendra and Paul Linnet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supertato</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M/NGS/NGS/NGS/NGS/NGS/NGS/NGS/NGS/NGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Evil Pea/Pepper/Pear/Melon/Carrot/Lolly;the other/Cucumber/Broccoli/Tomato/Aubergine</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The Lighthouse Keeper's Lunch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ronda and David Armitage</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mr. Grinling; Mr Grinling</t>
-  </si>
-  <si>
-    <t xml:space="preserve">F/M/M/M/M/M</t>
-  </si>
-  <si>
     <t xml:space="preserve">Mrs Grinling/Hamish/Fred/Tom/Bert/Seagulls</t>
   </si>
   <si>
@@ -1357,7 +1360,7 @@
     <t xml:space="preserve">Vivian French </t>
   </si>
   <si>
-    <t xml:space="preserve">M/H/NGS/NGS/NGS</t>
+    <t xml:space="preserve">M/M/NGS/NGS/NGS</t>
   </si>
   <si>
     <t xml:space="preserve">H/H/NH/NH /NH</t>
@@ -1399,13 +1402,13 @@
     <t xml:space="preserve">the farmer</t>
   </si>
   <si>
-    <t xml:space="preserve">F/M/M/F/NGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H/H/NH/NH/NH</t>
-  </si>
-  <si>
-    <t xml:space="preserve">farmer's wife;his wife/Jack/dog/cat/bird</t>
+    <t xml:space="preserve">F/M/M/F/NGS/NGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H/H/NH/NH/NH/H</t>
+  </si>
+  <si>
+    <t xml:space="preserve">farmer's wife;his wife/Jack/dog/cat/bird/parents</t>
   </si>
   <si>
     <t xml:space="preserve">The Very Lazy Ladybird</t>
@@ -2764,7 +2767,7 @@
     <t xml:space="preserve">NH/H/H</t>
   </si>
   <si>
-    <t xml:space="preserve">Worry/teacher/the boy;boy</t>
+    <t xml:space="preserve">Worry/teacher/boy;the boy</t>
   </si>
   <si>
     <t xml:space="preserve">Invisible Isabelle</t>
@@ -3060,10 +3063,10 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <sz val="6.4"/>
+      <color rgb="FF4C4C4C"/>
+      <name val="Ubuntu"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="9"/>
@@ -3160,12 +3163,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -3246,7 +3249,7 @@
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
-      <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="FF4C4C4C"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -3259,8 +3262,8 @@
   </sheetPr>
   <dimension ref="A1:Q207"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M53" colorId="64" zoomScale="274" zoomScaleNormal="274" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M59" activeCellId="0" sqref="M59"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L80" colorId="64" zoomScale="274" zoomScaleNormal="274" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M88" activeCellId="0" sqref="M88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.45" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7069,10 +7072,10 @@
         <v>394</v>
       </c>
       <c r="N76" s="2" t="s">
-        <v>334</v>
+        <v>395</v>
       </c>
       <c r="O76" s="2" t="s">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="P76" s="2"/>
       <c r="Q76" s="2" t="n">
@@ -7084,7 +7087,7 @@
         <v>76</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="C77" s="2" t="s">
         <v>186</v>
@@ -7110,19 +7113,19 @@
         <v>26</v>
       </c>
       <c r="L77" s="2" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="M77" s="2" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="N77" s="2" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="O77" s="2" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="P77" s="2" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="Q77" s="2" t="n">
         <v>1983</v>
@@ -7133,10 +7136,10 @@
         <v>77</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="D78" s="2" t="s">
         <v>19</v>
@@ -7163,19 +7166,19 @@
         <v>32</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="M78" s="2" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="N78" s="2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="O78" s="2" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="P78" s="2" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="Q78" s="2" t="n">
         <v>2016</v>
@@ -7186,7 +7189,7 @@
         <v>78</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="C79" s="2" t="s">
         <v>337</v>
@@ -7216,19 +7219,19 @@
         <v>26</v>
       </c>
       <c r="L79" s="2" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="M79" s="2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="N79" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O79" s="2" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="P79" s="2" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="Q79" s="2" t="n">
         <v>2000</v>
@@ -7239,10 +7242,10 @@
         <v>79</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="D80" s="2" t="s">
         <v>19</v>
@@ -7269,7 +7272,7 @@
         <v>26</v>
       </c>
       <c r="L80" s="2" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="M80" s="2" t="s">
         <v>40</v>
@@ -7278,7 +7281,7 @@
         <v>26</v>
       </c>
       <c r="O80" s="2" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="P80" s="2"/>
       <c r="Q80" s="2" t="n">
@@ -7290,7 +7293,7 @@
         <v>80</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C81" s="2" t="s">
         <v>186</v>
@@ -7320,19 +7323,19 @@
         <v>26</v>
       </c>
       <c r="L81" s="2" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="M81" s="2" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="N81" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O81" s="2" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="P81" s="2" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="Q81" s="2" t="n">
         <v>1980</v>
@@ -7343,7 +7346,7 @@
         <v>81</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C82" s="2" t="s">
         <v>186</v>
@@ -7367,25 +7370,25 @@
         <v>24</v>
       </c>
       <c r="J82" s="2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="K82" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L82" s="2" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="M82" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="N82" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O82" s="2" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="P82" s="2" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="Q82" s="2" t="n">
         <v>1987</v>
@@ -7396,7 +7399,7 @@
         <v>82</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="C83" s="2" t="s">
         <v>337</v>
@@ -7426,7 +7429,7 @@
         <v>26</v>
       </c>
       <c r="L83" s="2" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="M83" s="2" t="s">
         <v>40</v>
@@ -7435,7 +7438,7 @@
         <v>26</v>
       </c>
       <c r="O83" s="2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="P83" s="2"/>
       <c r="Q83" s="2" t="n">
@@ -7447,10 +7450,10 @@
         <v>83</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="D84" s="2" t="s">
         <v>19</v>
@@ -7473,16 +7476,16 @@
         <v>32</v>
       </c>
       <c r="L84" s="2" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="M84" s="2" t="s">
         <v>73</v>
       </c>
       <c r="N84" s="2" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="O84" s="2" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="P84" s="2"/>
       <c r="Q84" s="2" t="n">
@@ -7494,13 +7497,13 @@
         <v>84</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="C85" s="2" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="E85" s="2" t="n">
         <v>2.99</v>
@@ -7524,7 +7527,7 @@
         <v>26</v>
       </c>
       <c r="L85" s="2" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="M85" s="2" t="s">
         <v>40</v>
@@ -7533,10 +7536,10 @@
         <v>26</v>
       </c>
       <c r="O85" s="2" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="P85" s="2" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="Q85" s="2" t="n">
         <v>2016</v>
@@ -7547,10 +7550,10 @@
         <v>85</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="D86" s="2" t="s">
         <v>28</v>
@@ -7580,16 +7583,16 @@
         <v>111</v>
       </c>
       <c r="M86" s="2" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="N86" s="2" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="O86" s="2" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="P86" s="2" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="Q86" s="2" t="n">
         <v>2008</v>
@@ -7600,10 +7603,10 @@
         <v>86</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>78</v>
@@ -7622,15 +7625,15 @@
       <c r="P87" s="1"/>
       <c r="Q87" s="1"/>
     </row>
-    <row r="88" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="0" t="n">
         <v>87</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="D88" s="2" t="s">
         <v>78</v>
@@ -7653,16 +7656,16 @@
         <v>45</v>
       </c>
       <c r="L88" s="2" t="s">
-        <v>453</v>
-      </c>
-      <c r="M88" s="2" t="s">
-        <v>26</v>
+        <v>454</v>
+      </c>
+      <c r="M88" s="6" t="s">
+        <v>455</v>
       </c>
       <c r="N88" s="2" t="s">
-        <v>454</v>
+        <v>26</v>
       </c>
       <c r="O88" s="2" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="P88" s="2"/>
       <c r="Q88" s="2" t="n">
@@ -7674,10 +7677,10 @@
         <v>88</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="D89" s="2" t="s">
         <v>28</v>
@@ -7704,16 +7707,16 @@
         <v>32</v>
       </c>
       <c r="L89" s="2" t="s">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="M89" s="2" t="s">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="N89" s="2" t="s">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="O89" s="2" t="s">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="P89" s="2"/>
       <c r="Q89" s="2" t="n">
@@ -7725,10 +7728,10 @@
         <v>89</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="D90" s="2" t="s">
         <v>258</v>
@@ -7755,16 +7758,16 @@
         <v>26</v>
       </c>
       <c r="L90" s="2" t="s">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="M90" s="2" t="s">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="N90" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O90" s="2" t="s">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="P90" s="2"/>
       <c r="Q90" s="2" t="n">
@@ -7776,10 +7779,10 @@
         <v>90</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>467</v>
+        <v>468</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="D91" s="2" t="s">
         <v>258</v>
@@ -7806,16 +7809,16 @@
         <v>26</v>
       </c>
       <c r="L91" s="2" t="s">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="M91" s="2" t="s">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="N91" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O91" s="2" t="s">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="P91" s="2"/>
       <c r="Q91" s="2" t="n">
@@ -7827,10 +7830,10 @@
         <v>91</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="D92" s="2" t="s">
         <v>28</v>
@@ -7853,7 +7856,7 @@
         <v>45</v>
       </c>
       <c r="L92" s="2" t="s">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="M92" s="2"/>
       <c r="N92" s="2"/>
@@ -7868,10 +7871,10 @@
         <v>92</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C93" s="2" t="s">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="D93" s="2" t="s">
         <v>19</v>
@@ -7897,16 +7900,16 @@
       <c r="K93" s="4"/>
       <c r="L93" s="2"/>
       <c r="M93" s="4" t="s">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="N93" s="4" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="O93" s="4" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="P93" s="2" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="Q93" s="2" t="n">
         <v>1991</v>
@@ -7917,10 +7920,10 @@
         <v>93</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="C94" s="2" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="D94" s="2" t="s">
         <v>19</v>
@@ -7947,16 +7950,16 @@
         <v>26</v>
       </c>
       <c r="L94" s="2" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="M94" s="2" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="N94" s="2" t="s">
         <v>32</v>
       </c>
       <c r="O94" s="2" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="P94" s="2"/>
       <c r="Q94" s="2" t="n">
@@ -7968,10 +7971,10 @@
         <v>94</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="C95" s="2" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D95" s="2" t="s">
         <v>19</v>
@@ -7994,13 +7997,13 @@
         <v>26</v>
       </c>
       <c r="L95" s="2" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="M95" s="2"/>
       <c r="N95" s="2"/>
       <c r="O95" s="2"/>
       <c r="P95" s="2" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="Q95" s="2" t="n">
         <v>1969</v>
@@ -8011,10 +8014,10 @@
         <v>95</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C96" s="2" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="D96" s="2" t="s">
         <v>28</v>
@@ -8041,7 +8044,7 @@
         <v>26</v>
       </c>
       <c r="L96" s="2" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="M96" s="2" t="s">
         <v>58</v>
@@ -8050,10 +8053,10 @@
         <v>45</v>
       </c>
       <c r="O96" s="2" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="P96" s="2" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="Q96" s="2" t="n">
         <v>2004</v>
@@ -8064,10 +8067,10 @@
         <v>96</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C97" s="2" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D97" s="2" t="s">
         <v>19</v>
@@ -8094,19 +8097,19 @@
         <v>26</v>
       </c>
       <c r="L97" s="2" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="M97" s="2" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="N97" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O97" s="2" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="P97" s="2" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="Q97" s="2" t="n">
         <v>1984</v>
@@ -8117,10 +8120,10 @@
         <v>97</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="D98" s="2" t="s">
         <v>206</v>
@@ -8143,7 +8146,7 @@
         <v>45</v>
       </c>
       <c r="L98" s="2" t="s">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="M98" s="2" t="s">
         <v>311</v>
@@ -8152,7 +8155,7 @@
         <v>45</v>
       </c>
       <c r="O98" s="2" t="s">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="P98" s="2"/>
       <c r="Q98" s="2" t="n">
@@ -8164,10 +8167,10 @@
         <v>98</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="C99" s="2" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="D99" s="2" t="s">
         <v>55</v>
@@ -8194,7 +8197,7 @@
         <v>26</v>
       </c>
       <c r="L99" s="2" t="s">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="M99" s="2" t="s">
         <v>40</v>
@@ -8203,7 +8206,7 @@
         <v>26</v>
       </c>
       <c r="O99" s="2" t="s">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="P99" s="2"/>
       <c r="Q99" s="2" t="n">
@@ -8215,10 +8218,10 @@
         <v>99</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>507</v>
+        <v>508</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="D100" s="2" t="s">
         <v>28</v>
@@ -8245,7 +8248,7 @@
         <v>26</v>
       </c>
       <c r="L100" s="2" t="s">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="M100" s="2" t="s">
         <v>169</v>
@@ -8254,7 +8257,7 @@
         <v>45</v>
       </c>
       <c r="O100" s="2" t="s">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="P100" s="2"/>
       <c r="Q100" s="2" t="n">
@@ -8266,10 +8269,10 @@
         <v>100</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="C101" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D101" s="2" t="s">
         <v>19</v>
@@ -8292,16 +8295,16 @@
         <v>32</v>
       </c>
       <c r="L101" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="M101" s="2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="N101" s="2" t="s">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="O101" s="2" t="s">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="P101" s="2"/>
       <c r="Q101" s="2" t="n">
@@ -8313,10 +8316,10 @@
         <v>101</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="C102" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D102" s="2" t="s">
         <v>19</v>
@@ -8339,7 +8342,7 @@
         <v>32</v>
       </c>
       <c r="L102" s="2" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="M102" s="2" t="s">
         <v>58</v>
@@ -8348,7 +8351,7 @@
         <v>369</v>
       </c>
       <c r="O102" s="2" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="P102" s="2"/>
       <c r="Q102" s="2" t="n">
@@ -8360,10 +8363,10 @@
         <v>102</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="C103" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D103" s="2" t="s">
         <v>19</v>
@@ -8386,16 +8389,16 @@
         <v>32</v>
       </c>
       <c r="L103" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="M103" s="2" t="s">
         <v>34</v>
       </c>
       <c r="N103" s="2" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="O103" s="2" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="P103" s="2"/>
       <c r="Q103" s="2" t="n">
@@ -8407,10 +8410,10 @@
         <v>103</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="D104" s="2" t="s">
         <v>19</v>
@@ -8433,16 +8436,16 @@
         <v>32</v>
       </c>
       <c r="L104" s="2" t="s">
-        <v>513</v>
+        <v>514</v>
       </c>
       <c r="M104" s="2" t="s">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="N104" s="2" t="s">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="O104" s="2" t="s">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="P104" s="2"/>
       <c r="Q104" s="2" t="n">
@@ -8454,10 +8457,10 @@
         <v>104</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="D105" s="2" t="s">
         <v>73</v>
@@ -8466,7 +8469,7 @@
         <v>3.06</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="G105" s="2" t="n">
         <v>6</v>
@@ -8484,16 +8487,16 @@
         <v>32</v>
       </c>
       <c r="L105" s="2" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="M105" s="2" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="N105" s="2" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="O105" s="2" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="P105" s="2"/>
       <c r="Q105" s="2" t="n">
@@ -8505,10 +8508,10 @@
         <v>105</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="D106" s="2" t="s">
         <v>257</v>
@@ -8535,7 +8538,7 @@
         <v>26</v>
       </c>
       <c r="L106" s="2" t="s">
-        <v>536</v>
+        <v>537</v>
       </c>
       <c r="M106" s="2" t="s">
         <v>58</v>
@@ -8544,7 +8547,7 @@
         <v>26</v>
       </c>
       <c r="O106" s="2" t="s">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="P106" s="2"/>
       <c r="Q106" s="2" t="n">
@@ -8556,10 +8559,10 @@
         <v>106</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="C107" s="2" t="s">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="D107" s="2" t="s">
         <v>206</v>
@@ -8586,16 +8589,16 @@
         <v>26</v>
       </c>
       <c r="L107" s="2" t="s">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="M107" s="2" t="s">
-        <v>541</v>
+        <v>542</v>
       </c>
       <c r="N107" s="2" t="s">
         <v>45</v>
       </c>
       <c r="O107" s="2" t="s">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="P107" s="2"/>
       <c r="Q107" s="2" t="n">
@@ -8607,13 +8610,13 @@
         <v>107</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="D108" s="2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="E108" s="2" t="n">
         <v>3.5</v>
@@ -8637,19 +8640,19 @@
         <v>26</v>
       </c>
       <c r="L108" s="2" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="M108" s="2" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="N108" s="2" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="O108" s="2" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="P108" s="2" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="Q108" s="2" t="n">
         <v>2016</v>
@@ -8660,10 +8663,10 @@
         <v>108</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="D109" s="2" t="s">
         <v>19</v>
@@ -8686,19 +8689,19 @@
         <v>45</v>
       </c>
       <c r="L109" s="2" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="M109" s="2" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="N109" s="2" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="O109" s="2" t="s">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="P109" s="2" t="s">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="Q109" s="2" t="n">
         <v>2019</v>
@@ -8709,10 +8712,10 @@
         <v>109</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="D110" s="2" t="s">
         <v>19</v>
@@ -8735,16 +8738,16 @@
         <v>26</v>
       </c>
       <c r="L110" s="2" t="s">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="M110" s="2" t="s">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="N110" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O110" s="2" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="P110" s="2"/>
       <c r="Q110" s="2" t="n">
@@ -8756,10 +8759,10 @@
         <v>110</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="C111" s="2" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="D111" s="2" t="s">
         <v>206</v>
@@ -8786,16 +8789,16 @@
         <v>26</v>
       </c>
       <c r="L111" s="2" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
       <c r="M111" s="2" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="N111" s="2" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="O111" s="2" t="s">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="P111" s="2"/>
       <c r="Q111" s="2" t="n">
@@ -8807,10 +8810,10 @@
         <v>111</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="D112" s="2" t="s">
         <v>258</v>
@@ -8837,19 +8840,19 @@
         <v>26</v>
       </c>
       <c r="L112" s="2" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="M112" s="2" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="N112" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O112" s="2" t="s">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="P112" s="2" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="Q112" s="2" t="n">
         <v>2017</v>
@@ -8860,10 +8863,10 @@
         <v>112</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="D113" s="2" t="s">
         <v>258</v>
@@ -8893,13 +8896,13 @@
         <v>100</v>
       </c>
       <c r="M113" s="2" t="s">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="N113" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O113" s="2" t="s">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="P113" s="2"/>
       <c r="Q113" s="2" t="n">
@@ -8911,10 +8914,10 @@
         <v>113</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="D114" s="2" t="s">
         <v>258</v>
@@ -8941,16 +8944,16 @@
         <v>26</v>
       </c>
       <c r="L114" s="2" t="s">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="M114" s="2" t="s">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="N114" s="2" t="s">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="O114" s="2" t="s">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="P114" s="2"/>
       <c r="Q114" s="2" t="n">
@@ -8962,10 +8965,10 @@
         <v>114</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="D115" s="2" t="s">
         <v>55</v>
@@ -8992,7 +8995,7 @@
         <v>369</v>
       </c>
       <c r="L115" s="2" t="s">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="M115" s="2" t="s">
         <v>28</v>
@@ -9001,7 +9004,7 @@
         <v>26</v>
       </c>
       <c r="O115" s="2" t="s">
-        <v>586</v>
+        <v>587</v>
       </c>
       <c r="P115" s="2"/>
       <c r="Q115" s="2" t="n">
@@ -9013,10 +9016,10 @@
         <v>115</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="D116" s="2" t="s">
         <v>28</v>
@@ -9025,7 +9028,7 @@
         <v>2.99</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="G116" s="2" t="n">
         <v>7</v>
@@ -9037,18 +9040,18 @@
         <v>77</v>
       </c>
       <c r="J116" s="2" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="K116" s="2"/>
       <c r="L116" s="2"/>
       <c r="M116" s="2" t="s">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="N116" s="2" t="s">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="O116" s="2" t="s">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="P116" s="2"/>
       <c r="Q116" s="2" t="n">
@@ -9060,10 +9063,10 @@
         <v>116</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>594</v>
+        <v>595</v>
       </c>
       <c r="D117" s="2" t="s">
         <v>19</v>
@@ -9091,7 +9094,7 @@
         <v>26</v>
       </c>
       <c r="O117" s="2" t="s">
-        <v>595</v>
+        <v>596</v>
       </c>
       <c r="P117" s="2"/>
       <c r="Q117" s="2" t="n">
@@ -9103,7 +9106,7 @@
         <v>117</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>596</v>
+        <v>597</v>
       </c>
       <c r="C118" s="2" t="s">
         <v>376</v>
@@ -9129,19 +9132,19 @@
         <v>32</v>
       </c>
       <c r="L118" s="2" t="s">
-        <v>597</v>
+        <v>598</v>
       </c>
       <c r="M118" s="4" t="s">
-        <v>598</v>
+        <v>599</v>
       </c>
       <c r="N118" s="4" t="s">
-        <v>599</v>
+        <v>600</v>
       </c>
       <c r="O118" s="4" t="s">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="P118" s="4" t="s">
-        <v>601</v>
+        <v>602</v>
       </c>
       <c r="Q118" s="2" t="n">
         <v>2014</v>
@@ -9152,10 +9155,10 @@
         <v>118</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>602</v>
+        <v>603</v>
       </c>
       <c r="C119" s="2" t="s">
-        <v>603</v>
+        <v>604</v>
       </c>
       <c r="D119" s="2" t="s">
         <v>28</v>
@@ -9180,16 +9183,16 @@
         <v>26</v>
       </c>
       <c r="L119" s="2" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="M119" s="2" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="N119" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O119" s="2" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="P119" s="2"/>
       <c r="Q119" s="2" t="n">
@@ -9201,10 +9204,10 @@
         <v>119</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="D120" s="2" t="s">
         <v>28</v>
@@ -9231,16 +9234,16 @@
         <v>45</v>
       </c>
       <c r="L120" s="4" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="M120" s="2" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="N120" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O120" s="4" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="P120" s="2"/>
       <c r="Q120" s="2" t="n">
@@ -9252,10 +9255,10 @@
         <v>120</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="D121" s="2" t="s">
         <v>19</v>
@@ -9278,19 +9281,19 @@
         <v>45</v>
       </c>
       <c r="L121" s="2" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="M121" s="2" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="N121" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O121" s="2" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="P121" s="2" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="Q121" s="2" t="n">
         <v>2020</v>
@@ -9301,10 +9304,10 @@
         <v>121</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>19</v>
@@ -9331,19 +9334,19 @@
         <v>26</v>
       </c>
       <c r="L122" s="2" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
       <c r="M122" s="2" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
       <c r="N122" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O122" s="2" t="s">
-        <v>622</v>
-      </c>
-      <c r="P122" s="6" t="s">
         <v>623</v>
+      </c>
+      <c r="P122" s="7" t="s">
+        <v>624</v>
       </c>
       <c r="Q122" s="2" t="n">
         <v>2017</v>
@@ -9354,10 +9357,10 @@
         <v>122</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>624</v>
+        <v>625</v>
       </c>
       <c r="C123" s="2" t="s">
-        <v>625</v>
+        <v>626</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>28</v>
@@ -9383,16 +9386,16 @@
       <c r="K123" s="2"/>
       <c r="L123" s="2"/>
       <c r="M123" s="2" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
       <c r="N123" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O123" s="2" t="s">
-        <v>627</v>
+        <v>628</v>
       </c>
       <c r="P123" s="2" t="s">
-        <v>628</v>
+        <v>629</v>
       </c>
       <c r="Q123" s="2" t="n">
         <v>2000</v>
@@ -9403,10 +9406,10 @@
         <v>123</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>629</v>
+        <v>630</v>
       </c>
       <c r="C124" s="2" t="s">
-        <v>630</v>
+        <v>631</v>
       </c>
       <c r="D124" s="2" t="s">
         <v>28</v>
@@ -9433,19 +9436,19 @@
         <v>32</v>
       </c>
       <c r="L124" s="2" t="s">
-        <v>631</v>
+        <v>632</v>
       </c>
       <c r="M124" s="2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="N124" s="2" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="O124" s="2" t="s">
-        <v>633</v>
+        <v>634</v>
       </c>
       <c r="P124" s="2" t="s">
-        <v>634</v>
+        <v>635</v>
       </c>
       <c r="Q124" s="2" t="n">
         <v>2010</v>
@@ -9456,10 +9459,10 @@
         <v>124</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>635</v>
+        <v>636</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>636</v>
+        <v>637</v>
       </c>
       <c r="D125" s="2" t="s">
         <v>258</v>
@@ -9482,19 +9485,19 @@
         <v>32</v>
       </c>
       <c r="L125" s="2" t="s">
-        <v>637</v>
+        <v>638</v>
       </c>
       <c r="M125" s="2" t="s">
-        <v>638</v>
+        <v>639</v>
       </c>
       <c r="N125" s="2" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="O125" s="2" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="P125" s="4" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="Q125" s="2" t="n">
         <v>2019</v>
@@ -9505,10 +9508,10 @@
         <v>125</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="D126" s="2" t="s">
         <v>28</v>
@@ -9535,16 +9538,16 @@
         <v>26</v>
       </c>
       <c r="L126" s="2" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="M126" s="2" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="N126" s="2" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="O126" s="2" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="P126" s="2"/>
       <c r="Q126" s="2" t="n">
@@ -9556,10 +9559,10 @@
         <v>126</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="C127" s="2" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="D127" s="2" t="s">
         <v>206</v>
@@ -9568,7 +9571,7 @@
         <v>2.58</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>529</v>
+        <v>530</v>
       </c>
       <c r="G127" s="2" t="n">
         <v>6</v>
@@ -9586,19 +9589,19 @@
         <v>26</v>
       </c>
       <c r="L127" s="2" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="M127" s="2" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="N127" s="2" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="O127" s="2" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="P127" s="2" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="Q127" s="2" t="n">
         <v>2019</v>
@@ -9609,10 +9612,10 @@
         <v>127</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="D128" s="2" t="s">
         <v>19</v>
@@ -9633,7 +9636,7 @@
         <v>24</v>
       </c>
       <c r="J128" s="2" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="K128" s="2"/>
       <c r="L128" s="2" t="s">
@@ -9652,10 +9655,10 @@
         <v>128</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="C129" s="2" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="D129" s="2" t="s">
         <v>28</v>
@@ -9678,16 +9681,16 @@
         <v>32</v>
       </c>
       <c r="L129" s="2" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="M129" s="2" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="N129" s="2" t="s">
-        <v>632</v>
+        <v>633</v>
       </c>
       <c r="O129" s="2" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="P129" s="2"/>
       <c r="Q129" s="2" t="n">
@@ -9699,10 +9702,10 @@
         <v>129</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="D130" s="2" t="s">
         <v>19</v>
@@ -9723,7 +9726,7 @@
         <v>77</v>
       </c>
       <c r="J130" s="2" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="K130" s="2" t="s">
         <v>361</v>
@@ -9736,10 +9739,10 @@
         <v>26</v>
       </c>
       <c r="O130" s="2" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="P130" s="2" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="Q130" s="2" t="n">
         <v>2017</v>
@@ -9750,10 +9753,10 @@
         <v>130</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="D131" s="2" t="s">
         <v>258</v>
@@ -9774,13 +9777,13 @@
         <v>24</v>
       </c>
       <c r="J131" s="2" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="K131" s="2" t="s">
         <v>26</v>
       </c>
       <c r="L131" s="2" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="M131" s="2"/>
       <c r="N131" s="2"/>
@@ -9795,10 +9798,10 @@
         <v>131</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="D132" s="2" t="s">
         <v>19</v>
@@ -9821,16 +9824,16 @@
         <v>45</v>
       </c>
       <c r="L132" s="2" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="M132" s="2" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="N132" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O132" s="2" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="P132" s="2"/>
       <c r="Q132" s="2" t="n">
@@ -9842,10 +9845,10 @@
         <v>132</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="D133" s="2" t="s">
         <v>28</v>
@@ -9868,16 +9871,16 @@
         <v>32</v>
       </c>
       <c r="L133" s="2" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="M133" s="2" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="N133" s="2" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="O133" s="2" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="P133" s="2"/>
       <c r="Q133" s="2" t="n">
@@ -9889,10 +9892,10 @@
         <v>133</v>
       </c>
       <c r="B134" s="2" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="D134" s="2" t="s">
         <v>19</v>
@@ -9919,16 +9922,16 @@
         <v>26</v>
       </c>
       <c r="L134" s="2" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
       <c r="M134" s="2" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
       <c r="N134" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O134" s="2" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
       <c r="P134" s="2"/>
       <c r="Q134" s="2" t="n">
@@ -9940,10 +9943,10 @@
         <v>134</v>
       </c>
       <c r="B135" s="2" t="s">
-        <v>687</v>
+        <v>688</v>
       </c>
       <c r="C135" s="2" t="s">
-        <v>688</v>
+        <v>689</v>
       </c>
       <c r="D135" s="2" t="s">
         <v>28</v>
@@ -9960,7 +9963,7 @@
         <v>77</v>
       </c>
       <c r="J135" s="2" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="K135" s="2"/>
       <c r="L135" s="2"/>
@@ -9968,10 +9971,10 @@
         <v>40</v>
       </c>
       <c r="N135" s="2" t="s">
-        <v>689</v>
+        <v>690</v>
       </c>
       <c r="O135" s="2" t="s">
-        <v>690</v>
+        <v>691</v>
       </c>
       <c r="P135" s="2"/>
       <c r="Q135" s="2" t="n">
@@ -9983,10 +9986,10 @@
         <v>135</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="D136" s="2" t="s">
         <v>258</v>
@@ -10013,16 +10016,16 @@
         <v>26</v>
       </c>
       <c r="L136" s="2" t="s">
-        <v>693</v>
+        <v>694</v>
       </c>
       <c r="M136" s="2" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="N136" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O136" s="2" t="s">
-        <v>694</v>
+        <v>695</v>
       </c>
       <c r="P136" s="2"/>
       <c r="Q136" s="2" t="n">
@@ -10034,10 +10037,10 @@
         <v>136</v>
       </c>
       <c r="B137" s="2" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
       <c r="D137" s="2" t="s">
         <v>258</v>
@@ -10060,16 +10063,16 @@
         <v>26</v>
       </c>
       <c r="L137" s="2" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
       <c r="M137" s="2" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
       <c r="N137" s="2" t="s">
         <v>45</v>
       </c>
       <c r="O137" s="2" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
       <c r="P137" s="2"/>
       <c r="Q137" s="2" t="n">
@@ -10081,10 +10084,10 @@
         <v>137</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="D138" s="2" t="s">
         <v>258</v>
@@ -10106,13 +10109,13 @@
       <c r="K138" s="2"/>
       <c r="L138" s="2"/>
       <c r="M138" s="2" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
       <c r="N138" s="2" t="s">
-        <v>702</v>
-      </c>
-      <c r="O138" s="7" t="s">
         <v>703</v>
+      </c>
+      <c r="O138" s="2" t="s">
+        <v>704</v>
       </c>
       <c r="P138" s="2"/>
       <c r="Q138" s="2" t="n">
@@ -10124,10 +10127,10 @@
         <v>138</v>
       </c>
       <c r="B139" s="2" t="s">
-        <v>704</v>
+        <v>705</v>
       </c>
       <c r="C139" s="2" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="D139" s="2" t="s">
         <v>258</v>
@@ -10157,13 +10160,13 @@
         <v>41</v>
       </c>
       <c r="M139" s="2" t="s">
-        <v>705</v>
+        <v>706</v>
       </c>
       <c r="N139" s="2" t="s">
         <v>32</v>
       </c>
       <c r="O139" s="2" t="s">
-        <v>706</v>
+        <v>707</v>
       </c>
       <c r="P139" s="2"/>
       <c r="Q139" s="2" t="n">
@@ -10175,10 +10178,10 @@
         <v>139</v>
       </c>
       <c r="B140" s="2" t="s">
-        <v>707</v>
+        <v>708</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="D140" s="2" t="s">
         <v>258</v>
@@ -10205,19 +10208,19 @@
         <v>32</v>
       </c>
       <c r="L140" s="2" t="s">
-        <v>709</v>
+        <v>710</v>
       </c>
       <c r="M140" s="2" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="N140" s="2" t="s">
-        <v>711</v>
+        <v>712</v>
       </c>
       <c r="O140" s="2" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="P140" s="2" t="s">
-        <v>713</v>
+        <v>714</v>
       </c>
       <c r="Q140" s="2" t="n">
         <v>2013</v>
@@ -10228,10 +10231,10 @@
         <v>140</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>714</v>
+        <v>715</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>715</v>
+        <v>716</v>
       </c>
       <c r="D141" s="2" t="s">
         <v>28</v>
@@ -10254,19 +10257,19 @@
         <v>32</v>
       </c>
       <c r="L141" s="2" t="s">
-        <v>716</v>
+        <v>717</v>
       </c>
       <c r="M141" s="2" t="s">
-        <v>717</v>
+        <v>718</v>
       </c>
       <c r="N141" s="2" t="s">
-        <v>718</v>
+        <v>719</v>
       </c>
       <c r="O141" s="2" t="s">
-        <v>719</v>
+        <v>720</v>
       </c>
       <c r="P141" s="2" t="s">
-        <v>720</v>
+        <v>721</v>
       </c>
       <c r="Q141" s="2" t="n">
         <v>2018</v>
@@ -10277,10 +10280,10 @@
         <v>141</v>
       </c>
       <c r="B142" s="2" t="s">
-        <v>721</v>
+        <v>722</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>722</v>
+        <v>723</v>
       </c>
       <c r="D142" s="2" t="s">
         <v>19</v>
@@ -10303,19 +10306,19 @@
         <v>32</v>
       </c>
       <c r="L142" s="2" t="s">
-        <v>723</v>
+        <v>724</v>
       </c>
       <c r="M142" s="2" t="s">
-        <v>724</v>
+        <v>725</v>
       </c>
       <c r="N142" s="2" t="s">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="O142" s="2" t="s">
-        <v>726</v>
+        <v>727</v>
       </c>
       <c r="P142" s="2" t="s">
-        <v>727</v>
+        <v>728</v>
       </c>
       <c r="Q142" s="2" t="n">
         <v>2014</v>
@@ -10326,10 +10329,10 @@
         <v>142</v>
       </c>
       <c r="B143" s="2" t="s">
-        <v>728</v>
+        <v>729</v>
       </c>
       <c r="C143" s="2" t="s">
-        <v>729</v>
+        <v>730</v>
       </c>
       <c r="D143" s="2" t="s">
         <v>28</v>
@@ -10352,16 +10355,16 @@
         <v>26</v>
       </c>
       <c r="L143" s="2" t="s">
-        <v>730</v>
+        <v>731</v>
       </c>
       <c r="M143" s="2" t="s">
-        <v>731</v>
+        <v>732</v>
       </c>
       <c r="N143" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O143" s="2" t="s">
-        <v>732</v>
+        <v>733</v>
       </c>
       <c r="P143" s="2"/>
       <c r="Q143" s="2" t="n">
@@ -10373,10 +10376,10 @@
         <v>143</v>
       </c>
       <c r="B144" s="2" t="s">
-        <v>733</v>
+        <v>734</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>734</v>
+        <v>735</v>
       </c>
       <c r="D144" s="2" t="s">
         <v>28</v>
@@ -10403,7 +10406,7 @@
         <v>26</v>
       </c>
       <c r="L144" s="2" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="M144" s="2" t="s">
         <v>40</v>
@@ -10412,7 +10415,7 @@
         <v>26</v>
       </c>
       <c r="O144" s="2" t="s">
-        <v>736</v>
+        <v>737</v>
       </c>
       <c r="P144" s="2"/>
       <c r="Q144" s="2" t="n">
@@ -10424,10 +10427,10 @@
         <v>144</v>
       </c>
       <c r="B145" s="2" t="s">
-        <v>737</v>
+        <v>738</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="D145" s="2" t="s">
         <v>258</v>
@@ -10454,16 +10457,16 @@
         <v>32</v>
       </c>
       <c r="L145" s="2" t="s">
-        <v>738</v>
+        <v>739</v>
       </c>
       <c r="M145" s="2" t="s">
-        <v>739</v>
+        <v>740</v>
       </c>
       <c r="N145" s="2" t="s">
-        <v>740</v>
+        <v>741</v>
       </c>
       <c r="O145" s="2" t="s">
-        <v>741</v>
+        <v>742</v>
       </c>
       <c r="P145" s="2"/>
       <c r="Q145" s="2" t="n">
@@ -10475,10 +10478,10 @@
         <v>145</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>742</v>
+        <v>743</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="D146" s="2" t="s">
         <v>258</v>
@@ -10504,13 +10507,13 @@
       <c r="K146" s="2"/>
       <c r="L146" s="2"/>
       <c r="M146" s="2" t="s">
-        <v>710</v>
+        <v>711</v>
       </c>
       <c r="N146" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O146" s="2" t="s">
-        <v>743</v>
+        <v>744</v>
       </c>
       <c r="P146" s="2"/>
       <c r="Q146" s="2" t="n">
@@ -10522,10 +10525,10 @@
         <v>146</v>
       </c>
       <c r="B147" s="2" t="s">
-        <v>744</v>
+        <v>745</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>708</v>
+        <v>709</v>
       </c>
       <c r="D147" s="2" t="s">
         <v>258</v>
@@ -10551,13 +10554,13 @@
         <v>111</v>
       </c>
       <c r="M147" s="2" t="s">
-        <v>745</v>
+        <v>746</v>
       </c>
       <c r="N147" s="2" t="s">
-        <v>746</v>
+        <v>747</v>
       </c>
       <c r="O147" s="2" t="s">
-        <v>747</v>
+        <v>748</v>
       </c>
       <c r="P147" s="2"/>
       <c r="Q147" s="2" t="n">
@@ -10569,10 +10572,10 @@
         <v>147</v>
       </c>
       <c r="B148" s="2" t="s">
-        <v>748</v>
+        <v>749</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>749</v>
+        <v>750</v>
       </c>
       <c r="D148" s="2" t="s">
         <v>28</v>
@@ -10595,7 +10598,7 @@
         <v>26</v>
       </c>
       <c r="L148" s="2" t="s">
-        <v>750</v>
+        <v>751</v>
       </c>
       <c r="M148" s="2" t="s">
         <v>206</v>
@@ -10604,7 +10607,7 @@
         <v>383</v>
       </c>
       <c r="O148" s="2" t="s">
-        <v>751</v>
+        <v>752</v>
       </c>
       <c r="P148" s="2"/>
       <c r="Q148" s="2" t="n">
@@ -10616,10 +10619,10 @@
         <v>148</v>
       </c>
       <c r="B149" s="2" t="s">
-        <v>752</v>
+        <v>753</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>753</v>
+        <v>754</v>
       </c>
       <c r="D149" s="2" t="s">
         <v>206</v>
@@ -10642,19 +10645,19 @@
         <v>32</v>
       </c>
       <c r="L149" s="2" t="s">
-        <v>754</v>
+        <v>755</v>
       </c>
       <c r="M149" s="2" t="s">
         <v>258</v>
       </c>
       <c r="N149" s="2" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="O149" s="2" t="s">
-        <v>755</v>
+        <v>756</v>
       </c>
       <c r="P149" s="2" t="s">
-        <v>756</v>
+        <v>757</v>
       </c>
       <c r="Q149" s="2" t="n">
         <v>2020</v>
@@ -10665,10 +10668,10 @@
         <v>149</v>
       </c>
       <c r="B150" s="2" t="s">
-        <v>757</v>
+        <v>758</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>758</v>
+        <v>759</v>
       </c>
       <c r="D150" s="2" t="s">
         <v>28</v>
@@ -10691,16 +10694,16 @@
         <v>32</v>
       </c>
       <c r="L150" s="2" t="s">
-        <v>759</v>
+        <v>760</v>
       </c>
       <c r="M150" s="2" t="s">
-        <v>760</v>
+        <v>761</v>
       </c>
       <c r="N150" s="2" t="s">
-        <v>761</v>
+        <v>762</v>
       </c>
       <c r="O150" s="2" t="s">
-        <v>762</v>
+        <v>763</v>
       </c>
       <c r="P150" s="2"/>
       <c r="Q150" s="2" t="n">
@@ -10712,10 +10715,10 @@
         <v>150</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>763</v>
+        <v>764</v>
       </c>
       <c r="C151" s="2" t="s">
-        <v>764</v>
+        <v>765</v>
       </c>
       <c r="D151" s="2" t="s">
         <v>19</v>
@@ -10732,7 +10735,7 @@
         <v>77</v>
       </c>
       <c r="J151" s="2" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="K151" s="2"/>
       <c r="L151" s="2"/>
@@ -10749,7 +10752,7 @@
         <v>151</v>
       </c>
       <c r="B152" s="2" t="s">
-        <v>765</v>
+        <v>766</v>
       </c>
       <c r="C152" s="2" t="s">
         <v>246</v>
@@ -10775,19 +10778,19 @@
         <v>369</v>
       </c>
       <c r="L152" s="2" t="s">
-        <v>766</v>
+        <v>767</v>
       </c>
       <c r="M152" s="2" t="s">
-        <v>767</v>
+        <v>768</v>
       </c>
       <c r="N152" s="2" t="s">
-        <v>768</v>
+        <v>769</v>
       </c>
       <c r="O152" s="2" t="s">
-        <v>769</v>
+        <v>770</v>
       </c>
       <c r="P152" s="2" t="s">
-        <v>770</v>
+        <v>771</v>
       </c>
       <c r="Q152" s="2" t="n">
         <v>2018</v>
@@ -10798,7 +10801,7 @@
         <v>152</v>
       </c>
       <c r="B153" s="2" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="C153" s="2" t="s">
         <v>246</v>
@@ -10824,19 +10827,19 @@
         <v>32</v>
       </c>
       <c r="L153" s="2" t="s">
-        <v>771</v>
+        <v>772</v>
       </c>
       <c r="M153" s="2" t="s">
-        <v>772</v>
+        <v>773</v>
       </c>
       <c r="N153" s="2" t="s">
-        <v>773</v>
+        <v>774</v>
       </c>
       <c r="O153" s="2" t="s">
-        <v>774</v>
+        <v>775</v>
       </c>
       <c r="P153" s="2" t="s">
-        <v>775</v>
+        <v>776</v>
       </c>
       <c r="Q153" s="2" t="n">
         <v>2010</v>
@@ -10847,7 +10850,7 @@
         <v>153</v>
       </c>
       <c r="B154" s="2" t="s">
-        <v>776</v>
+        <v>777</v>
       </c>
       <c r="C154" s="2" t="s">
         <v>246</v>
@@ -10873,16 +10876,16 @@
         <v>45</v>
       </c>
       <c r="L154" s="2" t="s">
-        <v>777</v>
+        <v>778</v>
       </c>
       <c r="M154" s="2" t="s">
-        <v>778</v>
+        <v>779</v>
       </c>
       <c r="N154" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O154" s="4" t="s">
-        <v>779</v>
+        <v>780</v>
       </c>
       <c r="P154" s="2"/>
       <c r="Q154" s="2" t="n">
@@ -10894,7 +10897,7 @@
         <v>154</v>
       </c>
       <c r="B155" s="2" t="s">
-        <v>780</v>
+        <v>781</v>
       </c>
       <c r="C155" s="2" t="s">
         <v>246</v>
@@ -10920,16 +10923,16 @@
         <v>26</v>
       </c>
       <c r="L155" s="2" t="s">
-        <v>781</v>
+        <v>782</v>
       </c>
       <c r="M155" s="2" t="s">
-        <v>782</v>
+        <v>783</v>
       </c>
       <c r="N155" s="2" t="s">
         <v>130</v>
       </c>
       <c r="O155" s="2" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
       <c r="P155" s="2"/>
       <c r="Q155" s="2" t="n">
@@ -10941,7 +10944,7 @@
         <v>155</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>784</v>
+        <v>785</v>
       </c>
       <c r="C156" s="2" t="s">
         <v>246</v>
@@ -10967,16 +10970,16 @@
         <v>26</v>
       </c>
       <c r="L156" s="2" t="s">
-        <v>785</v>
+        <v>786</v>
       </c>
       <c r="M156" s="2" t="s">
-        <v>786</v>
+        <v>787</v>
       </c>
       <c r="N156" s="2" t="s">
-        <v>787</v>
+        <v>788</v>
       </c>
       <c r="O156" s="2" t="s">
-        <v>788</v>
+        <v>789</v>
       </c>
       <c r="P156" s="2"/>
       <c r="Q156" s="2" t="n">
@@ -10988,7 +10991,7 @@
         <v>156</v>
       </c>
       <c r="B157" s="2" t="s">
-        <v>789</v>
+        <v>790</v>
       </c>
       <c r="C157" s="2" t="s">
         <v>246</v>
@@ -11014,16 +11017,16 @@
         <v>26</v>
       </c>
       <c r="L157" s="2" t="s">
-        <v>790</v>
+        <v>791</v>
       </c>
       <c r="M157" s="2" t="s">
-        <v>791</v>
+        <v>792</v>
       </c>
       <c r="N157" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O157" s="4" t="s">
-        <v>792</v>
+        <v>793</v>
       </c>
       <c r="P157" s="2"/>
       <c r="Q157" s="2" t="n">
@@ -11035,7 +11038,7 @@
         <v>157</v>
       </c>
       <c r="B158" s="2" t="s">
-        <v>793</v>
+        <v>794</v>
       </c>
       <c r="C158" s="2" t="s">
         <v>246</v>
@@ -11061,16 +11064,16 @@
         <v>26</v>
       </c>
       <c r="L158" s="2" t="s">
-        <v>794</v>
+        <v>795</v>
       </c>
       <c r="M158" s="2" t="s">
-        <v>795</v>
+        <v>796</v>
       </c>
       <c r="N158" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O158" s="2" t="s">
-        <v>796</v>
+        <v>797</v>
       </c>
       <c r="P158" s="2"/>
       <c r="Q158" s="2" t="n">
@@ -11082,7 +11085,7 @@
         <v>158</v>
       </c>
       <c r="B159" s="2" t="s">
-        <v>797</v>
+        <v>798</v>
       </c>
       <c r="C159" s="2" t="s">
         <v>246</v>
@@ -11108,16 +11111,16 @@
         <v>26</v>
       </c>
       <c r="L159" s="2" t="s">
-        <v>798</v>
+        <v>799</v>
       </c>
       <c r="M159" s="2" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="N159" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O159" s="2" t="s">
-        <v>800</v>
+        <v>801</v>
       </c>
       <c r="P159" s="2"/>
       <c r="Q159" s="2" t="n">
@@ -11129,7 +11132,7 @@
         <v>159</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>801</v>
+        <v>802</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>246</v>
@@ -11149,7 +11152,7 @@
         <v>77</v>
       </c>
       <c r="J160" s="2" t="s">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="K160" s="2"/>
       <c r="L160" s="2"/>
@@ -11160,7 +11163,7 @@
         <v>26</v>
       </c>
       <c r="O160" s="2" t="s">
-        <v>802</v>
+        <v>803</v>
       </c>
       <c r="P160" s="2"/>
       <c r="Q160" s="2" t="n">
@@ -11172,7 +11175,7 @@
         <v>160</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>803</v>
+        <v>804</v>
       </c>
       <c r="C161" s="2" t="s">
         <v>246</v>
@@ -11198,16 +11201,16 @@
         <v>32</v>
       </c>
       <c r="L161" s="2" t="s">
-        <v>804</v>
+        <v>805</v>
       </c>
       <c r="M161" s="2" t="s">
-        <v>805</v>
+        <v>806</v>
       </c>
       <c r="N161" s="2" t="s">
         <v>32</v>
       </c>
       <c r="O161" s="2" t="s">
-        <v>806</v>
+        <v>807</v>
       </c>
       <c r="P161" s="2"/>
       <c r="Q161" s="2" t="n">
@@ -11219,7 +11222,7 @@
         <v>161</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>807</v>
+        <v>808</v>
       </c>
       <c r="C162" s="2" t="s">
         <v>246</v>
@@ -11245,16 +11248,16 @@
         <v>45</v>
       </c>
       <c r="L162" s="2" t="s">
-        <v>808</v>
+        <v>809</v>
       </c>
       <c r="M162" s="2" t="s">
         <v>154</v>
       </c>
       <c r="N162" s="2" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="O162" s="2" t="s">
-        <v>809</v>
+        <v>810</v>
       </c>
       <c r="P162" s="2"/>
       <c r="Q162" s="2" t="n">
@@ -11266,7 +11269,7 @@
         <v>162</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>810</v>
+        <v>811</v>
       </c>
       <c r="C163" s="2" t="s">
         <v>246</v>
@@ -11292,16 +11295,16 @@
         <v>26</v>
       </c>
       <c r="L163" s="2" t="s">
-        <v>811</v>
+        <v>812</v>
       </c>
       <c r="M163" s="2" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="N163" s="2" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="O163" s="2" t="s">
-        <v>814</v>
+        <v>815</v>
       </c>
       <c r="P163" s="2"/>
       <c r="Q163" s="2" t="n">
@@ -11313,7 +11316,7 @@
         <v>163</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="C164" s="2" t="s">
         <v>246</v>
@@ -11339,19 +11342,19 @@
         <v>26</v>
       </c>
       <c r="L164" s="2" t="s">
-        <v>815</v>
+        <v>816</v>
       </c>
       <c r="M164" s="2" t="s">
-        <v>816</v>
+        <v>817</v>
       </c>
       <c r="N164" s="2" t="s">
-        <v>817</v>
+        <v>818</v>
       </c>
       <c r="O164" s="2" t="s">
-        <v>818</v>
+        <v>819</v>
       </c>
       <c r="P164" s="2" t="s">
-        <v>819</v>
+        <v>820</v>
       </c>
       <c r="Q164" s="2" t="n">
         <v>2010</v>
@@ -11362,7 +11365,7 @@
         <v>164</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>820</v>
+        <v>821</v>
       </c>
       <c r="C165" s="2" t="s">
         <v>246</v>
@@ -11388,16 +11391,16 @@
         <v>45</v>
       </c>
       <c r="L165" s="2" t="s">
-        <v>821</v>
+        <v>822</v>
       </c>
       <c r="M165" s="2" t="s">
-        <v>822</v>
+        <v>823</v>
       </c>
       <c r="N165" s="2" t="s">
-        <v>823</v>
+        <v>824</v>
       </c>
       <c r="O165" s="2" t="s">
-        <v>824</v>
+        <v>825</v>
       </c>
       <c r="P165" s="2"/>
       <c r="Q165" s="2" t="n">
@@ -11409,7 +11412,7 @@
         <v>165</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>825</v>
+        <v>826</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>246</v>
@@ -11435,16 +11438,16 @@
         <v>32</v>
       </c>
       <c r="L166" s="2" t="s">
-        <v>826</v>
+        <v>827</v>
       </c>
       <c r="M166" s="2" t="s">
-        <v>827</v>
+        <v>828</v>
       </c>
       <c r="N166" s="2" t="s">
-        <v>828</v>
+        <v>829</v>
       </c>
       <c r="O166" s="2" t="s">
-        <v>829</v>
+        <v>830</v>
       </c>
       <c r="P166" s="2"/>
       <c r="Q166" s="2" t="n">
@@ -11456,7 +11459,7 @@
         <v>166</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>830</v>
+        <v>831</v>
       </c>
       <c r="C167" s="2" t="s">
         <v>246</v>
@@ -11482,19 +11485,19 @@
         <v>32</v>
       </c>
       <c r="L167" s="2" t="s">
-        <v>831</v>
+        <v>832</v>
       </c>
       <c r="M167" s="2" t="s">
-        <v>832</v>
+        <v>833</v>
       </c>
       <c r="N167" s="2" t="s">
-        <v>833</v>
+        <v>834</v>
       </c>
       <c r="O167" s="2" t="s">
-        <v>834</v>
+        <v>835</v>
       </c>
       <c r="P167" s="2" t="s">
-        <v>835</v>
+        <v>836</v>
       </c>
       <c r="Q167" s="2" t="n">
         <v>2012</v>
@@ -11534,13 +11537,13 @@
         <v>388</v>
       </c>
       <c r="M168" s="2" t="s">
-        <v>836</v>
+        <v>837</v>
       </c>
       <c r="N168" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O168" s="2" t="s">
-        <v>837</v>
+        <v>838</v>
       </c>
       <c r="P168" s="2"/>
       <c r="Q168" s="2" t="n">
@@ -11552,7 +11555,7 @@
         <v>168</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>838</v>
+        <v>839</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>387</v>
@@ -11578,19 +11581,19 @@
         <v>45</v>
       </c>
       <c r="L169" s="2" t="s">
-        <v>839</v>
+        <v>840</v>
       </c>
       <c r="M169" s="2" t="s">
-        <v>840</v>
+        <v>841</v>
       </c>
       <c r="N169" s="2" t="s">
-        <v>841</v>
+        <v>842</v>
       </c>
       <c r="O169" s="2" t="s">
-        <v>842</v>
+        <v>843</v>
       </c>
       <c r="P169" s="2" t="s">
-        <v>843</v>
+        <v>844</v>
       </c>
       <c r="Q169" s="2" t="n">
         <v>2016</v>
@@ -11601,10 +11604,10 @@
         <v>169</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="C170" s="2" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="D170" s="2" t="s">
         <v>28</v>
@@ -11627,19 +11630,19 @@
         <v>45</v>
       </c>
       <c r="L170" s="2" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="M170" s="2" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="N170" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O170" s="2" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
       <c r="P170" s="2" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="Q170" s="2" t="n">
         <v>2013</v>
@@ -11650,10 +11653,10 @@
         <v>170</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>28</v>
@@ -11676,16 +11679,16 @@
         <v>45</v>
       </c>
       <c r="L171" s="2" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="M171" s="2" t="s">
-        <v>852</v>
+        <v>853</v>
       </c>
       <c r="N171" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O171" s="2" t="s">
-        <v>853</v>
+        <v>854</v>
       </c>
       <c r="P171" s="2"/>
       <c r="Q171" s="2" t="n">
@@ -11697,10 +11700,10 @@
         <v>171</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>854</v>
+        <v>855</v>
       </c>
       <c r="C172" s="2" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="D172" s="2" t="s">
         <v>28</v>
@@ -11726,13 +11729,13 @@
         <v>310</v>
       </c>
       <c r="M172" s="2" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="N172" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O172" s="2" t="s">
-        <v>855</v>
+        <v>856</v>
       </c>
       <c r="P172" s="2"/>
       <c r="Q172" s="2" t="n">
@@ -11744,10 +11747,10 @@
         <v>172</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>856</v>
+        <v>857</v>
       </c>
       <c r="C173" s="2" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="D173" s="2" t="s">
         <v>28</v>
@@ -11770,7 +11773,7 @@
         <v>45</v>
       </c>
       <c r="L173" s="2" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="M173" s="2" t="s">
         <v>58</v>
@@ -11779,7 +11782,7 @@
         <v>26</v>
       </c>
       <c r="O173" s="2" t="s">
-        <v>857</v>
+        <v>858</v>
       </c>
       <c r="P173" s="2"/>
       <c r="Q173" s="2" t="n">
@@ -11791,10 +11794,10 @@
         <v>173</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>858</v>
+        <v>859</v>
       </c>
       <c r="C174" s="2" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="D174" s="2" t="s">
         <v>28</v>
@@ -11817,7 +11820,7 @@
         <v>45</v>
       </c>
       <c r="L174" s="2" t="s">
-        <v>859</v>
+        <v>860</v>
       </c>
       <c r="M174" s="2" t="s">
         <v>73</v>
@@ -11826,7 +11829,7 @@
         <v>45</v>
       </c>
       <c r="O174" s="2" t="s">
-        <v>860</v>
+        <v>861</v>
       </c>
       <c r="P174" s="2"/>
       <c r="Q174" s="2" t="n">
@@ -11838,7 +11841,7 @@
         <v>174</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>861</v>
+        <v>862</v>
       </c>
       <c r="C175" s="2" t="s">
         <v>387</v>
@@ -11864,16 +11867,16 @@
         <v>26</v>
       </c>
       <c r="L175" s="2" t="s">
-        <v>862</v>
+        <v>863</v>
       </c>
       <c r="M175" s="2" t="s">
-        <v>863</v>
+        <v>864</v>
       </c>
       <c r="N175" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O175" s="2" t="s">
-        <v>864</v>
+        <v>865</v>
       </c>
       <c r="P175" s="2"/>
       <c r="Q175" s="2" t="n">
@@ -11885,10 +11888,10 @@
         <v>175</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>865</v>
+        <v>866</v>
       </c>
       <c r="C176" s="2" t="s">
-        <v>866</v>
+        <v>867</v>
       </c>
       <c r="D176" s="2" t="s">
         <v>28</v>
@@ -11911,16 +11914,16 @@
         <v>45</v>
       </c>
       <c r="L176" s="2" t="s">
-        <v>867</v>
+        <v>868</v>
       </c>
       <c r="M176" s="2" t="s">
-        <v>868</v>
+        <v>869</v>
       </c>
       <c r="N176" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O176" s="2" t="s">
-        <v>869</v>
+        <v>870</v>
       </c>
       <c r="P176" s="2"/>
       <c r="Q176" s="2" t="n">
@@ -11932,10 +11935,10 @@
         <v>176</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>870</v>
+        <v>871</v>
       </c>
       <c r="C177" s="2" t="s">
-        <v>871</v>
+        <v>872</v>
       </c>
       <c r="D177" s="2" t="s">
         <v>28</v>
@@ -11957,16 +11960,16 @@
       <c r="K177" s="2"/>
       <c r="L177" s="2"/>
       <c r="M177" s="2" t="s">
-        <v>872</v>
+        <v>873</v>
       </c>
       <c r="N177" s="2" t="s">
         <v>32</v>
       </c>
       <c r="O177" s="2" t="s">
-        <v>873</v>
+        <v>874</v>
       </c>
       <c r="P177" s="2" t="s">
-        <v>874</v>
+        <v>875</v>
       </c>
       <c r="Q177" s="2" t="n">
         <v>2019</v>
@@ -11977,10 +11980,10 @@
         <v>177</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>875</v>
+        <v>876</v>
       </c>
       <c r="C178" s="2" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="D178" s="2" t="s">
         <v>28</v>
@@ -12003,16 +12006,16 @@
         <v>32</v>
       </c>
       <c r="L178" s="2" t="s">
-        <v>877</v>
+        <v>878</v>
       </c>
       <c r="M178" s="2" t="s">
-        <v>878</v>
+        <v>879</v>
       </c>
       <c r="N178" s="2" t="s">
         <v>32</v>
       </c>
       <c r="O178" s="2" t="s">
-        <v>879</v>
+        <v>880</v>
       </c>
       <c r="P178" s="2"/>
       <c r="Q178" s="2" t="n">
@@ -12024,10 +12027,10 @@
         <v>178</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>880</v>
+        <v>881</v>
       </c>
       <c r="C179" s="2" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="D179" s="2" t="s">
         <v>28</v>
@@ -12050,16 +12053,16 @@
         <v>32</v>
       </c>
       <c r="L179" s="2" t="s">
-        <v>881</v>
+        <v>882</v>
       </c>
       <c r="M179" s="2" t="s">
-        <v>882</v>
+        <v>883</v>
       </c>
       <c r="N179" s="2" t="s">
-        <v>883</v>
+        <v>884</v>
       </c>
       <c r="O179" s="2" t="s">
-        <v>884</v>
+        <v>885</v>
       </c>
       <c r="P179" s="2"/>
       <c r="Q179" s="2" t="n">
@@ -12071,10 +12074,10 @@
         <v>179</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>885</v>
+        <v>886</v>
       </c>
       <c r="C180" s="2" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="D180" s="2" t="s">
         <v>28</v>
@@ -12097,19 +12100,19 @@
         <v>32</v>
       </c>
       <c r="L180" s="2" t="s">
-        <v>886</v>
+        <v>887</v>
       </c>
       <c r="M180" s="2" t="s">
-        <v>887</v>
+        <v>888</v>
       </c>
       <c r="N180" s="2" t="s">
-        <v>888</v>
+        <v>889</v>
       </c>
       <c r="O180" s="2" t="s">
-        <v>889</v>
+        <v>890</v>
       </c>
       <c r="P180" s="2" t="s">
-        <v>890</v>
+        <v>891</v>
       </c>
       <c r="Q180" s="2" t="n">
         <v>2019</v>
@@ -12120,10 +12123,10 @@
         <v>180</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>891</v>
+        <v>892</v>
       </c>
       <c r="C181" s="2" t="s">
-        <v>892</v>
+        <v>893</v>
       </c>
       <c r="D181" s="2" t="s">
         <v>28</v>
@@ -12150,16 +12153,16 @@
         <v>45</v>
       </c>
       <c r="L181" s="2" t="s">
-        <v>893</v>
+        <v>894</v>
       </c>
       <c r="M181" s="2" t="s">
-        <v>894</v>
+        <v>895</v>
       </c>
       <c r="N181" s="2" t="s">
-        <v>895</v>
+        <v>896</v>
       </c>
       <c r="O181" s="2" t="s">
-        <v>896</v>
+        <v>897</v>
       </c>
       <c r="P181" s="2"/>
       <c r="Q181" s="2" t="n">
@@ -12171,10 +12174,10 @@
         <v>181</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>897</v>
+        <v>898</v>
       </c>
       <c r="C182" s="2" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="D182" s="2" t="s">
         <v>258</v>
@@ -12201,19 +12204,19 @@
         <v>26</v>
       </c>
       <c r="L182" s="2" t="s">
-        <v>899</v>
+        <v>900</v>
       </c>
       <c r="M182" s="2" t="s">
-        <v>900</v>
+        <v>901</v>
       </c>
       <c r="N182" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O182" s="2" t="s">
-        <v>901</v>
+        <v>902</v>
       </c>
       <c r="P182" s="2" t="s">
-        <v>902</v>
+        <v>903</v>
       </c>
       <c r="Q182" s="2" t="n">
         <v>2014</v>
@@ -12224,17 +12227,17 @@
         <v>182</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>903</v>
+        <v>904</v>
       </c>
       <c r="C183" s="2" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="D183" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E183" s="2"/>
       <c r="F183" s="2" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="G183" s="2" t="n">
         <v>6</v>
@@ -12252,16 +12255,16 @@
         <v>45</v>
       </c>
       <c r="L183" s="2" t="s">
-        <v>906</v>
+        <v>907</v>
       </c>
       <c r="M183" s="2" t="s">
-        <v>907</v>
+        <v>908</v>
       </c>
       <c r="N183" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O183" s="2" t="s">
-        <v>908</v>
+        <v>909</v>
       </c>
       <c r="P183" s="2"/>
       <c r="Q183" s="2" t="n">
@@ -12273,10 +12276,10 @@
         <v>183</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>909</v>
+        <v>910</v>
       </c>
       <c r="C184" s="2" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="D184" s="2" t="s">
         <v>19</v>
@@ -12299,16 +12302,16 @@
         <v>32</v>
       </c>
       <c r="L184" s="2" t="s">
-        <v>911</v>
+        <v>912</v>
       </c>
       <c r="M184" s="2" t="s">
-        <v>912</v>
+        <v>913</v>
       </c>
       <c r="N184" s="2" t="s">
-        <v>913</v>
+        <v>914</v>
       </c>
       <c r="O184" s="2" t="s">
-        <v>914</v>
+        <v>915</v>
       </c>
       <c r="P184" s="2"/>
       <c r="Q184" s="2" t="n">
@@ -12320,10 +12323,10 @@
         <v>184</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>915</v>
+        <v>916</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>916</v>
+        <v>917</v>
       </c>
       <c r="D185" s="1" t="s">
         <v>28</v>
@@ -12347,10 +12350,10 @@
         <v>185</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>917</v>
+        <v>918</v>
       </c>
       <c r="C186" s="2" t="s">
-        <v>918</v>
+        <v>919</v>
       </c>
       <c r="D186" s="2" t="s">
         <v>19</v>
@@ -12377,19 +12380,19 @@
         <v>369</v>
       </c>
       <c r="L186" s="2" t="s">
-        <v>919</v>
+        <v>920</v>
       </c>
       <c r="M186" s="2" t="s">
-        <v>920</v>
+        <v>921</v>
       </c>
       <c r="N186" s="2" t="s">
-        <v>921</v>
+        <v>922</v>
       </c>
       <c r="O186" s="2" t="s">
-        <v>922</v>
+        <v>923</v>
       </c>
       <c r="P186" s="2" t="s">
-        <v>923</v>
+        <v>924</v>
       </c>
       <c r="Q186" s="2" t="n">
         <v>2020</v>
@@ -12400,10 +12403,10 @@
         <v>186</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>924</v>
+        <v>925</v>
       </c>
       <c r="C187" s="2" t="s">
-        <v>925</v>
+        <v>926</v>
       </c>
       <c r="D187" s="2" t="s">
         <v>28</v>
@@ -12430,16 +12433,16 @@
         <v>26</v>
       </c>
       <c r="L187" s="2" t="s">
-        <v>926</v>
+        <v>927</v>
       </c>
       <c r="M187" s="2" t="s">
-        <v>927</v>
+        <v>928</v>
       </c>
       <c r="N187" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O187" s="2" t="s">
-        <v>928</v>
+        <v>929</v>
       </c>
       <c r="P187" s="2"/>
       <c r="Q187" s="2" t="n">
@@ -12451,10 +12454,10 @@
         <v>187</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>929</v>
+        <v>930</v>
       </c>
       <c r="C188" s="2" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="D188" s="2" t="s">
         <v>258</v>
@@ -12484,13 +12487,13 @@
         <v>352</v>
       </c>
       <c r="M188" s="2" t="s">
-        <v>930</v>
+        <v>931</v>
       </c>
       <c r="N188" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O188" s="2" t="s">
-        <v>931</v>
+        <v>932</v>
       </c>
       <c r="P188" s="2"/>
       <c r="Q188" s="2" t="n">
@@ -12502,10 +12505,10 @@
         <v>188</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>932</v>
+        <v>933</v>
       </c>
       <c r="C189" s="2" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="D189" s="2" t="s">
         <v>258</v>
@@ -12532,16 +12535,16 @@
         <v>26</v>
       </c>
       <c r="L189" s="2" t="s">
-        <v>933</v>
+        <v>934</v>
       </c>
       <c r="M189" s="2" t="s">
-        <v>934</v>
+        <v>935</v>
       </c>
       <c r="N189" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O189" s="2" t="s">
-        <v>935</v>
+        <v>936</v>
       </c>
       <c r="P189" s="2"/>
       <c r="Q189" s="2" t="n">
@@ -12553,10 +12556,10 @@
         <v>189</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>936</v>
+        <v>937</v>
       </c>
       <c r="C190" s="2" t="s">
-        <v>876</v>
+        <v>877</v>
       </c>
       <c r="D190" s="2" t="s">
         <v>28</v>
@@ -12579,16 +12582,16 @@
         <v>32</v>
       </c>
       <c r="L190" s="2" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="M190" s="2" t="s">
-        <v>938</v>
+        <v>939</v>
       </c>
       <c r="N190" s="2" t="s">
         <v>261</v>
       </c>
       <c r="O190" s="2" t="s">
-        <v>939</v>
+        <v>940</v>
       </c>
       <c r="P190" s="2"/>
       <c r="Q190" s="2" t="n">
@@ -12600,10 +12603,10 @@
         <v>190</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>940</v>
+        <v>941</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>258</v>
@@ -12630,19 +12633,19 @@
         <v>26</v>
       </c>
       <c r="L191" s="2" t="s">
-        <v>735</v>
+        <v>736</v>
       </c>
       <c r="M191" s="2" t="s">
-        <v>941</v>
+        <v>942</v>
       </c>
       <c r="N191" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O191" s="2" t="s">
-        <v>942</v>
+        <v>943</v>
       </c>
       <c r="P191" s="2" t="s">
-        <v>943</v>
+        <v>944</v>
       </c>
       <c r="Q191" s="2" t="n">
         <v>2016</v>
@@ -12653,10 +12656,10 @@
         <v>191</v>
       </c>
       <c r="B192" s="2" t="s">
-        <v>944</v>
+        <v>945</v>
       </c>
       <c r="C192" s="2" t="s">
-        <v>910</v>
+        <v>911</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>19</v>
@@ -12679,16 +12682,16 @@
         <v>361</v>
       </c>
       <c r="L192" s="2" t="s">
-        <v>945</v>
+        <v>946</v>
       </c>
       <c r="M192" s="2" t="s">
-        <v>946</v>
+        <v>947</v>
       </c>
       <c r="N192" s="2" t="s">
-        <v>947</v>
+        <v>948</v>
       </c>
       <c r="O192" s="2" t="s">
-        <v>948</v>
+        <v>949</v>
       </c>
       <c r="P192" s="2"/>
       <c r="Q192" s="2" t="n">
@@ -12700,17 +12703,17 @@
         <v>192</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>949</v>
+        <v>950</v>
       </c>
       <c r="C193" s="2" t="s">
-        <v>904</v>
+        <v>905</v>
       </c>
       <c r="D193" s="2" t="s">
         <v>28</v>
       </c>
       <c r="E193" s="2"/>
       <c r="F193" s="2" t="s">
-        <v>905</v>
+        <v>906</v>
       </c>
       <c r="G193" s="2" t="n">
         <v>8</v>
@@ -12728,19 +12731,19 @@
         <v>45</v>
       </c>
       <c r="L193" s="2" t="s">
-        <v>950</v>
+        <v>951</v>
       </c>
       <c r="M193" s="2" t="s">
-        <v>951</v>
+        <v>952</v>
       </c>
       <c r="N193" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O193" s="2" t="s">
-        <v>952</v>
+        <v>953</v>
       </c>
       <c r="P193" s="2" t="s">
-        <v>953</v>
+        <v>954</v>
       </c>
       <c r="Q193" s="2" t="n">
         <v>2012</v>
@@ -12751,10 +12754,10 @@
         <v>193</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>954</v>
+        <v>955</v>
       </c>
       <c r="C194" s="2" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="D194" s="2" t="s">
         <v>258</v>
@@ -12781,16 +12784,16 @@
         <v>26</v>
       </c>
       <c r="L194" s="2" t="s">
-        <v>955</v>
+        <v>956</v>
       </c>
       <c r="M194" s="2" t="s">
-        <v>956</v>
+        <v>957</v>
       </c>
       <c r="N194" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O194" s="2" t="s">
-        <v>957</v>
+        <v>958</v>
       </c>
       <c r="P194" s="2"/>
       <c r="Q194" s="2" t="n">
@@ -12802,10 +12805,10 @@
         <v>194</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>958</v>
+        <v>959</v>
       </c>
       <c r="C195" s="2" t="s">
-        <v>898</v>
+        <v>899</v>
       </c>
       <c r="D195" s="2" t="s">
         <v>258</v>
@@ -12832,16 +12835,16 @@
         <v>26</v>
       </c>
       <c r="L195" s="2" t="s">
-        <v>959</v>
+        <v>960</v>
       </c>
       <c r="M195" s="2" t="s">
-        <v>960</v>
+        <v>961</v>
       </c>
       <c r="N195" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O195" s="2" t="s">
-        <v>961</v>
+        <v>962</v>
       </c>
       <c r="P195" s="2"/>
       <c r="Q195" s="2" t="n">
@@ -12853,10 +12856,10 @@
         <v>195</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>962</v>
+        <v>963</v>
       </c>
       <c r="C196" s="2" t="s">
-        <v>963</v>
+        <v>964</v>
       </c>
       <c r="D196" s="2" t="s">
         <v>19</v>
@@ -12883,16 +12886,16 @@
         <v>45</v>
       </c>
       <c r="L196" s="2" t="s">
-        <v>964</v>
+        <v>965</v>
       </c>
       <c r="M196" s="2" t="s">
-        <v>965</v>
+        <v>966</v>
       </c>
       <c r="N196" s="2" t="s">
-        <v>966</v>
+        <v>967</v>
       </c>
       <c r="O196" s="2" t="s">
-        <v>967</v>
+        <v>968</v>
       </c>
       <c r="P196" s="2"/>
       <c r="Q196" s="2" t="n">
@@ -12904,10 +12907,10 @@
         <v>196</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>968</v>
+        <v>969</v>
       </c>
       <c r="C197" s="2" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="D197" s="2" t="s">
         <v>19</v>
@@ -12934,16 +12937,16 @@
         <v>45</v>
       </c>
       <c r="L197" s="2" t="s">
-        <v>970</v>
+        <v>971</v>
       </c>
       <c r="M197" s="2" t="s">
-        <v>971</v>
+        <v>972</v>
       </c>
       <c r="N197" s="2" t="s">
         <v>26</v>
       </c>
       <c r="O197" s="2" t="s">
-        <v>972</v>
+        <v>973</v>
       </c>
       <c r="P197" s="2"/>
       <c r="Q197" s="2" t="n">
@@ -12955,10 +12958,10 @@
         <v>197</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>973</v>
+        <v>974</v>
       </c>
       <c r="C198" s="2" t="s">
-        <v>974</v>
+        <v>975</v>
       </c>
       <c r="D198" s="2" t="s">
         <v>28</v>
@@ -12985,16 +12988,16 @@
         <v>32</v>
       </c>
       <c r="L198" s="2" t="s">
-        <v>975</v>
+        <v>976</v>
       </c>
       <c r="M198" s="2" t="s">
-        <v>976</v>
+        <v>977</v>
       </c>
       <c r="N198" s="2" t="s">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="O198" s="2" t="s">
-        <v>977</v>
+        <v>978</v>
       </c>
       <c r="P198" s="2"/>
       <c r="Q198" s="2" t="n">
@@ -13006,10 +13009,10 @@
         <v>198</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>978</v>
+        <v>979</v>
       </c>
       <c r="C199" s="2" t="s">
-        <v>979</v>
+        <v>980</v>
       </c>
       <c r="D199" s="2" t="s">
         <v>78</v>
@@ -13036,16 +13039,16 @@
         <v>45</v>
       </c>
       <c r="L199" s="2" t="s">
-        <v>980</v>
+        <v>981</v>
       </c>
       <c r="M199" s="2" t="s">
-        <v>981</v>
+        <v>982</v>
       </c>
       <c r="N199" s="2" t="s">
-        <v>982</v>
+        <v>983</v>
       </c>
       <c r="O199" s="2" t="s">
-        <v>983</v>
+        <v>984</v>
       </c>
       <c r="P199" s="2"/>
       <c r="Q199" s="2" t="n">
@@ -13057,10 +13060,10 @@
         <v>199</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="C200" s="2" t="s">
-        <v>985</v>
+        <v>986</v>
       </c>
       <c r="D200" s="2" t="s">
         <v>19</v>
@@ -13087,16 +13090,16 @@
         <v>361</v>
       </c>
       <c r="L200" s="2" t="s">
-        <v>984</v>
+        <v>985</v>
       </c>
       <c r="M200" s="2" t="s">
-        <v>986</v>
+        <v>987</v>
       </c>
       <c r="N200" s="2" t="s">
-        <v>987</v>
+        <v>988</v>
       </c>
       <c r="O200" s="2" t="s">
-        <v>988</v>
+        <v>989</v>
       </c>
       <c r="P200" s="2"/>
       <c r="Q200" s="2" t="n">
@@ -13108,10 +13111,10 @@
         <v>200</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>989</v>
+        <v>990</v>
       </c>
       <c r="C201" s="2" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="D201" s="2" t="s">
         <v>19</v>
@@ -13134,16 +13137,16 @@
         <v>32</v>
       </c>
       <c r="L201" s="2" t="s">
-        <v>937</v>
+        <v>938</v>
       </c>
       <c r="M201" s="2" t="s">
-        <v>990</v>
+        <v>991</v>
       </c>
       <c r="N201" s="2" t="s">
-        <v>991</v>
+        <v>992</v>
       </c>
       <c r="O201" s="2" t="s">
-        <v>992</v>
+        <v>993</v>
       </c>
       <c r="P201" s="2"/>
       <c r="Q201" s="2" t="n">
@@ -13155,10 +13158,10 @@
         <v>201</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>993</v>
+        <v>994</v>
       </c>
       <c r="C202" s="2" t="s">
-        <v>969</v>
+        <v>970</v>
       </c>
       <c r="D202" s="2" t="s">
         <v>19</v>
@@ -13175,13 +13178,13 @@
         <v>24</v>
       </c>
       <c r="J202" s="2" t="s">
-        <v>994</v>
+        <v>995</v>
       </c>
       <c r="K202" s="2" t="s">
-        <v>995</v>
+        <v>996</v>
       </c>
       <c r="L202" s="2" t="s">
-        <v>996</v>
+        <v>997</v>
       </c>
       <c r="M202" s="2" t="s">
         <v>19</v>
@@ -13190,7 +13193,7 @@
         <v>26</v>
       </c>
       <c r="O202" s="2" t="s">
-        <v>997</v>
+        <v>998</v>
       </c>
       <c r="P202" s="2"/>
       <c r="Q202" s="2" t="n">
@@ -13207,13 +13210,13 @@
     </row>
     <row r="206" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C206" s="10" t="s">
-        <v>998</v>
+        <v>999</v>
       </c>
       <c r="D206" s="10"/>
     </row>
     <row r="207" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C207" s="10" t="s">
-        <v>999</v>
+        <v>1000</v>
       </c>
       <c r="D207" s="10"/>
       <c r="E207" s="0" t="n">

</xml_diff>